<commit_message>
práce na katalogue makeru
</commit_message>
<xml_diff>
--- a/catalogue_manager/Sharepoint_databaze.xlsx
+++ b/catalogue_manager/Sharepoint_databaze.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakub.hlavacek.local\Desktop\JHV\Work\catalogue_manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BFB724C-14F4-445D-B58E-A2E4E4385083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5854EDA4-EDB7-4482-88EE-7784F287C2DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14595" yWindow="2295" windowWidth="23010" windowHeight="13650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kontrolery" sheetId="2" r:id="rId1"/>
@@ -217,9 +217,6 @@
     <t>FH-L551-10</t>
   </si>
   <si>
-    <t>FH-Lite controller, standard grade, box type, 4 camera, , W10 IoT Ente</t>
-  </si>
-  <si>
     <t xml:space="preserve">Keyence XG-X 
 </t>
   </si>
@@ -528,6 +525,9 @@
   </si>
   <si>
     <t>optika11</t>
+  </si>
+  <si>
+    <t>FH-Lite controller, standard grade, box type, 4 camera, , W10 IoT Ente</t>
   </si>
 </sst>
 </file>
@@ -924,8 +924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1207,7 +1207,7 @@
         <v>63</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>64</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -1223,7 +1223,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6243DA3-0875-4C03-8E69-F223C9363894}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
@@ -1241,90 +1241,90 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -1359,286 +1359,286 @@
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D1" s="12"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" t="s">
         <v>66</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>68</v>
-      </c>
       <c r="D2" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>71</v>
-      </c>
       <c r="D3" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" t="s">
         <v>72</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>74</v>
-      </c>
       <c r="D4" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" t="s">
         <v>75</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>77</v>
-      </c>
       <c r="D5" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>80</v>
-      </c>
       <c r="D6" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" t="s">
         <v>81</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>83</v>
-      </c>
       <c r="D7" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" t="s">
         <v>84</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>86</v>
-      </c>
       <c r="D8" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9" t="s">
         <v>87</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>89</v>
-      </c>
       <c r="D9" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B10" t="s">
         <v>90</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>92</v>
-      </c>
       <c r="D10" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" t="s">
         <v>93</v>
-      </c>
-      <c r="B11" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>94</v>
+      </c>
+      <c r="B12" t="s">
         <v>95</v>
-      </c>
-      <c r="B12" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13" t="s">
         <v>97</v>
-      </c>
-      <c r="B13" t="s">
-        <v>98</v>
       </c>
       <c r="C13" s="5"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>98</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>99</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>100</v>
+      </c>
+      <c r="B15" t="s">
         <v>101</v>
-      </c>
-      <c r="B15" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>102</v>
+      </c>
+      <c r="B16" t="s">
         <v>103</v>
-      </c>
-      <c r="B16" t="s">
-        <v>104</v>
       </c>
       <c r="C16" s="5"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>104</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>105</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>106</v>
+      </c>
+      <c r="B18" t="s">
         <v>107</v>
-      </c>
-      <c r="B18" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>108</v>
+      </c>
+      <c r="B19" t="s">
         <v>109</v>
-      </c>
-      <c r="B19" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>110</v>
+      </c>
+      <c r="B20" t="s">
         <v>111</v>
-      </c>
-      <c r="B20" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>112</v>
+      </c>
+      <c r="B21" t="s">
         <v>113</v>
-      </c>
-      <c r="B21" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>114</v>
+      </c>
+      <c r="B22" t="s">
         <v>115</v>
-      </c>
-      <c r="B22" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>116</v>
+      </c>
+      <c r="B23" t="s">
         <v>117</v>
-      </c>
-      <c r="B23" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>118</v>
+      </c>
+      <c r="B24" t="s">
         <v>119</v>
-      </c>
-      <c r="B24" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>120</v>
+      </c>
+      <c r="B25" t="s">
         <v>121</v>
-      </c>
-      <c r="B25" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>122</v>
+      </c>
+      <c r="B26" t="s">
         <v>123</v>
-      </c>
-      <c r="B26" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B27" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1760,118 +1760,118 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>128</v>
+      </c>
+      <c r="B10" t="s">
         <v>129</v>
       </c>
-      <c r="B10" t="s">
-        <v>130</v>
-      </c>
       <c r="C10" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>127</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>132</v>
+      </c>
+      <c r="B11" t="s">
         <v>133</v>
       </c>
-      <c r="B11" t="s">
-        <v>134</v>
-      </c>
       <c r="C11" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>131</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C12" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>135</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C13" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>137</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C14" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>139</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C15" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="D15" s="7" t="s">
         <v>141</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C16" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="D16" s="7" t="s">
         <v>143</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C17" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="D17" s="7" t="s">
         <v>145</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C18" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="D18" s="7" t="s">
         <v>147</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C19" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>149</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D20" s="7" t="s">
         <v>151</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D21" s="7" t="s">
         <v>153</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="22" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D22" s="7" t="s">
         <v>155</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="28" spans="3:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
export do xlsx, zprovozneni automaticke synchronizace se sharepointem, prvni verze 1.0
</commit_message>
<xml_diff>
--- a/catalogue_manager/Sharepoint_databaze.xlsx
+++ b/catalogue_manager/Sharepoint_databaze.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakub.hlavacek.local\Desktop\JHV\Work\catalogue_manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5854EDA4-EDB7-4482-88EE-7784F287C2DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{5854EDA4-EDB7-4482-88EE-7784F287C2DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E993AD4-A753-48D1-8614-FC36D62435F8}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kontrolery" sheetId="2" r:id="rId1"/>
@@ -18,12 +18,28 @@
     <sheet name="Kamery" sheetId="3" r:id="rId3"/>
     <sheet name="Přislušenství" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="449">
   <si>
     <t>Omron FZ/FH</t>
   </si>
@@ -31,30 +47,6 @@
     <t>Keyence XG-X</t>
   </si>
   <si>
-    <t>rozšíření kontroleru</t>
-  </si>
-  <si>
-    <t>SD karta</t>
-  </si>
-  <si>
-    <t>monitor</t>
-  </si>
-  <si>
-    <t>HDD</t>
-  </si>
-  <si>
-    <t>konzole</t>
-  </si>
-  <si>
-    <t>NAS</t>
-  </si>
-  <si>
-    <t>kamera</t>
-  </si>
-  <si>
-    <t>kabel ke kameře</t>
-  </si>
-  <si>
     <t>FH-2050</t>
   </si>
   <si>
@@ -215,6 +207,777 @@
   </si>
   <si>
     <t>FH-L551-10</t>
+  </si>
+  <si>
+    <t>FH-Lite controller, standard grade, box type, 4 camera, , W10 IoT Ente</t>
+  </si>
+  <si>
+    <t>optika1</t>
+  </si>
+  <si>
+    <t>3Z4S-LE SV-0814H</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, čočky, C montáž, pro kamery FZ-S_2M, FZ-S_5M3, FH-S_05R, FH-S_X05, FHV7H, ohnisková vzdálenost 8 mm, nejmenší vzdálenost 100mm, světelnost 1,4 až 16, maximální kompatiblní CCD čip 2/3" nebo 1"</t>
+  </si>
+  <si>
+    <t>optika2</t>
+  </si>
+  <si>
+    <t>3Z4S-LE SV-1214H</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, čočky, C montáž, pro kamery FZ-S_2M, FZ-S_5M3, FH-S_05R, FH-S_X05, FHV7H, ohnisková vzdálenost 12 mm, nejmenší vzdálenost 100mm, světelnost 1,4 až 16, maximální kompatiblní CCD čip 2/3" nebo 1"</t>
+  </si>
+  <si>
+    <t>optika3</t>
+  </si>
+  <si>
+    <t>3Z4S-LE SV-1614H</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, čočky, C montáž, pro kamery FZ-S_2M, FZ-S_5M3, FH-S_05R, FH-S_X05, FHV7H, ohnisková vzdálenost 16 mm, nejmenší vzdálenost 100mm, světelnost 1,4 až 16, maximální kompatiblní CCD čip 2/3" nebo 1"</t>
+  </si>
+  <si>
+    <t>optika4</t>
+  </si>
+  <si>
+    <t>3Z4S-LE SV-2514H</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, čočky, C montáž, pro kamery FZ-S_2M, FZ-S_5M3, FH-S_05R, FH-S_X05, FHV7H, ohnisková vzdálenost 25 mm, nejmenší vzdálenost 150mm, světelnost 1,4 až 16, maximální kompatiblní CCD čip 2/3" nebo 1"</t>
+  </si>
+  <si>
+    <t>optika5</t>
+  </si>
+  <si>
+    <t>3Z4S-LE SV-3514H</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, čočky, C montáž, pro kamery FZ-S_2M, FZ-S_5M3, FH-S_05R, FH-S_X05, FHV7H, ohnisková vzdálenost 35 mm, nejmenší vzdálenost 200mm, světelnost 1,4 až 16, maximální kompatiblní CCD čip 2/3" nebo 1"</t>
+  </si>
+  <si>
+    <t>optika6</t>
+  </si>
+  <si>
+    <t>3Z4S-LE SV-5014H</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, čočky, C montáž, pro kamery FZ-S_2M, FZ-S_5M3, FH-S_05R, FH-S_X05, FHV7H, ohnisková vzdálenost 50 mm, nejmenší vzdálenost 300mm, světelnost 1,4 až 16, maximální kompatiblní CCD čip 2/3" nebo 1"</t>
+  </si>
+  <si>
+    <t>optika7</t>
+  </si>
+  <si>
+    <t>3Z4S-LE SV-7525H</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, čočky, C montáž, pro kamery FZ-S_2M, FZ-S_5M3, FH-S_05R, FH-S_X05, FHV7H, ohnisková vzdálenost 75 mm, nejmenší vzdálenost 1200mm, světelnost 2,5 až zavřeno, maximální kompatiblní CCD čip 2/3" nebo 1", revize 1</t>
+  </si>
+  <si>
+    <t>optika8</t>
+  </si>
+  <si>
+    <t>3Z4S-LE SV-10028H</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, čočky, C montáž, pro kamery FZ-S_2M, FZ-S_5M3, FH-S_05R, FH-S_X05, FHV7H, ohnisková vzdálenost 100 mm, nejmenší vzdálenost 2000mm, světelnost 2,8 až zavřeno, maximální kompatiblní CCD čip 2/3" nebo 1", revize 1</t>
+  </si>
+  <si>
+    <t>optika9</t>
+  </si>
+  <si>
+    <t>optika10</t>
+  </si>
+  <si>
+    <t>3Z4S-LE VS-0618H1</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, čočky, C montáž, pro kamery FH-S_02, FH-S_04, ohnisková vzdálenost 6 mm, nejmenší vzdálenost 100mm, světelnost 1,8 až 16, maximální kompatiblní CCD čip 1", revize 1</t>
+  </si>
+  <si>
+    <t>optika11</t>
+  </si>
+  <si>
+    <t>3Z4S-LE VS-0814H1</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, čočky, C montáž, pro kamery FH-S_02, FH-S_04, ohnisková vzdálenost 8 mm, nejmenší vzdálenost 100mm, světelnost 1,4 až 16, maximální kompatiblní CCD čip 1"</t>
+  </si>
+  <si>
+    <t>optika12</t>
+  </si>
+  <si>
+    <t>3Z4S-LE VS-1214H1</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, čočky, C montáž, pro kamery FH-S_02, FH-S_04, ohnisková vzdálenost 12 mm, nejmenší vzdálenost 300mm, světelnost 1,4 až 16, maximální kompatiblní CCD čip 1", revize 1</t>
+  </si>
+  <si>
+    <t>optika13</t>
+  </si>
+  <si>
+    <t>3Z4S-LE VS-1614H1N</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, čočky, C montáž, pro kamery FH-S_02, FH-S_04, ohnisková vzdálenost 16 mm, nejmenší vzdálenost 300mm, světelnost 1,4 až 16, maximální kompatiblní CCD čip 1", revize 1</t>
+  </si>
+  <si>
+    <t>optika14</t>
+  </si>
+  <si>
+    <t>3Z4S-LE VS-2514H1</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, čočky, C montáž, pro kamery FH-S_02, FH-S_04, ohnisková vzdálenost 25 mm, nejmenší vzdálenost 300mm, světelnost 1,4 až 16, maximální kompatiblní CCD čip 1", revize 1</t>
+  </si>
+  <si>
+    <t>optika15</t>
+  </si>
+  <si>
+    <t>3Z4S-LE VS-3514H1</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, čočky, C montáž, pro kamery FH-S_02, FH-S_04, ohnisková vzdálenost 35 mm, nejmenší vzdálenost 300mm, světelnost 1,4 až 16, maximální kompatiblní CCD čip 1", revize 1</t>
+  </si>
+  <si>
+    <t>optika16</t>
+  </si>
+  <si>
+    <t>3Z4S-LE VS-5018H1</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, čočky, C montáž, pro kamery FH-S_02, FH-S_04, ohnisková vzdálenost 50 mm, nejmenší vzdálenost 500mm, světelnost 1,8 až 16, maximální kompatiblní CCD čip 1", revize 1</t>
+  </si>
+  <si>
+    <t>optika17</t>
+  </si>
+  <si>
+    <t>optika18</t>
+  </si>
+  <si>
+    <t>3Z4S-LE SV-03514V</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, čočky, C-montáž, pro kamery FZ-S, FZ-SH, FH-S, FH-S_X,FHV7H, ohnisková vzdálenost 3,5 mm, nejmenší vzdálenost 200mm, světelnost 1,4 až zavřeno, maximální kompatiblní CCD čip 1/3"</t>
+  </si>
+  <si>
+    <t>optika19</t>
+  </si>
+  <si>
+    <t>3Z4S-LE SV-04514V</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, čočky, C-montáž, pro kamery FZ-S, FZ-SH, FH-S, FH-S_X,FHV7H, ohnisková vzdálenost 4,5 mm, nejmenší vzdálenost 200mm, světelnost 1,4 až zavřeno, maximální kompatiblní CCD čip 1/3"</t>
+  </si>
+  <si>
+    <t>optika20</t>
+  </si>
+  <si>
+    <t>3Z4S-LE SV-0614H</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, čočky, C montáž, pro kamery FZ-S_2M, FZ-S_5M3, FH-S_05R, FH-S_X05, FHV7H, ohnisková vzdálenost 6 mm, nejmenší vzdálenost 100mm, světelnost 1,4 až 16, maximální kompatiblní CCD čip 2/3" nebo 1"</t>
+  </si>
+  <si>
+    <t>optika21</t>
+  </si>
+  <si>
+    <t>3Z4S-LE SV-0614V</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, čočky, C-montáž, pro kamery FZ-S, FZ-SH, FH-S, FH-S_X,FHV7H, ohnisková vzdálenost 6 mm, nejmenší vzdálenost 200mm, světelnost 1,4 až zavřeno, maximální kompatiblní CCD čip 1/3"</t>
+  </si>
+  <si>
+    <t>optika22</t>
+  </si>
+  <si>
+    <t>3Z4S-LE SV-0813V</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, čočky, C-montáž, pro kamery FZ-S, FZ-SH, FH-S, FH-S_X,FHV7H, ohnisková vzdálenost 8 mm, nejmenší vzdálenost 200mm, světelnost 1,3 až zavřeno, maximální kompatiblní CCD čip 1/3"</t>
+  </si>
+  <si>
+    <t>optika23</t>
+  </si>
+  <si>
+    <t>3Z4S-LE SV-1214V</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, čočky, C-montáž, pro kamery FZ-S, FZ-SH, FH-S, FH-S_X,FHV7H, ohnisková vzdálenost 12 mm, nejmenší vzdálenost 300mm, světelnost 1,4 až zavřeno, maximální kompatiblní CCD čip 1/3"</t>
+  </si>
+  <si>
+    <t>optika24</t>
+  </si>
+  <si>
+    <t>3Z4S-LE SV-1614V</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, čočky, C-montáž, pro kamery FZ-S, FZ-SH, FH-S, FH-S_X,FHV7H, ohnisková vzdálenost 16 mm, nejmenší vzdálenost 400mm, světelnost 1,4 až zavřeno, maximální kompatiblní CCD čip 1/3"</t>
+  </si>
+  <si>
+    <t>optika25</t>
+  </si>
+  <si>
+    <t>3Z4S-LE SV-2514V</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, čočky, C-montáž, pro kamery FZ-S, FZ-SH, FH-S, FH-S_X,FHV7H, ohnisková vzdálenost 25 mm, nejmenší vzdálenost 500mm, světelnost 1,4 až zavřeno, maximální kompatiblní CCD čip 1/3"</t>
+  </si>
+  <si>
+    <t>optika26</t>
+  </si>
+  <si>
+    <t>3Z4S-LE SV-3518V</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, čočky, C-montáž, pro kamery FZ-S, FZ-SH, FH-S, FH-S_X,FHV7H, ohnisková vzdálenost 35 mm, nejmenší vzdálenost 300mm, světelnost 1,8 až zavřeno, maximální kompatiblní CCD čip 1/3"</t>
+  </si>
+  <si>
+    <t>optika27</t>
+  </si>
+  <si>
+    <t>3Z4S-LE SV-5018V</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, čočky, C-montáž, pro kamery FZ-S, FZ-SH, FH-S, FH-S_X,FHV7H, ohnisková vzdálenost 50 mm, nejmenší vzdálenost 1000mm, světelnost 1,8 až zavřeno, maximální kompatiblní CCD čip 1/3"</t>
+  </si>
+  <si>
+    <t>optika28</t>
+  </si>
+  <si>
+    <t>3Z4S-LE SV-7527V</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, čočky, C-montáž, pro kamery FZ-S, FZ-SH, FH-S, FH-S_X,FHV7H, ohnisková vzdálenost 75 mm, nejmenší vzdálenost 1000mm, světelnost 2,7 až zavřeno, maximální kompatiblní CCD čip 1/3"</t>
+  </si>
+  <si>
+    <t>optika29</t>
+  </si>
+  <si>
+    <t>3Z4S-LE SV-10035V</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, čočky, C-montáž, pro kamery FZ-S, FZ-SH, FH-S, FH-S_X,FHV7H, ohnisková vzdálenost 100 mm, nejmenší vzdálenost 1000mm, světelnost 3,5 až zavřeno, maximální kompatiblní CCD čip 1/3"</t>
+  </si>
+  <si>
+    <t>optika30</t>
+  </si>
+  <si>
+    <t>optika31</t>
+  </si>
+  <si>
+    <t>3Z4S-LE SV-1.5X</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, zadní předsádka objektivů, 1,5x</t>
+  </si>
+  <si>
+    <t>optika32</t>
+  </si>
+  <si>
+    <t>3Z4S-LE SV-2.0X</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, zadní předsádka objektivů, 2,0x</t>
+  </si>
+  <si>
+    <t>optika33</t>
+  </si>
+  <si>
+    <t>3Z4S-LE SV-EXR</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, pro C-montáž, prodlužovací kroužek, sada 7 kroužků (40, 20, 10, 5, 2, 1, 0.5mm)</t>
+  </si>
+  <si>
+    <t>optika34</t>
+  </si>
+  <si>
+    <t>3Z4S-LE SV-EXR05</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, pro C-montáž, prodlužovací kroužek, 0,5 mm</t>
+  </si>
+  <si>
+    <t>optika35</t>
+  </si>
+  <si>
+    <t>3Z4S-LE SV-EXR1</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, pro C-montáž, prodlužovací kroužek, 1 mm</t>
+  </si>
+  <si>
+    <t>optika36</t>
+  </si>
+  <si>
+    <t>3Z4S-LE SV-EXR10</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, pro C-montáž, prodlužovací kroužek, 10 mm</t>
+  </si>
+  <si>
+    <t>optika37</t>
+  </si>
+  <si>
+    <t>3Z4S-LE SV-EXR15</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, pro C-montáž, prodlužovací kroužek, 15 mm</t>
+  </si>
+  <si>
+    <t>optika38</t>
+  </si>
+  <si>
+    <t>3Z4S-LE SV-EXR2</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, pro C-montáž, prodlužovací kroužek, 2 mm</t>
+  </si>
+  <si>
+    <t>optika39</t>
+  </si>
+  <si>
+    <t>3Z4S-LE SV-EXR20</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, pro C-montáž, prodlužovací kroužek, 20 mm</t>
+  </si>
+  <si>
+    <t>optika40</t>
+  </si>
+  <si>
+    <t>3Z4S-LE SV-EXR25</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, pro C-montáž, prodlužovací kroužek, 25 mm</t>
+  </si>
+  <si>
+    <t>optika41</t>
+  </si>
+  <si>
+    <t>3Z4S-LE SV-EXR30</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, pro C-montáž, prodlužovací kroužek, 30 mm</t>
+  </si>
+  <si>
+    <t>optika42</t>
+  </si>
+  <si>
+    <t>3Z4S-LE SV-EXR40</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, pro C-montáž, prodlužovací kroužek, 40 mm</t>
+  </si>
+  <si>
+    <t>optika43</t>
+  </si>
+  <si>
+    <t>3Z4S-LE SV-EXR5</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, pro C-montáž, prodlužovací kroužek, 5 mm</t>
+  </si>
+  <si>
+    <t>optika44</t>
+  </si>
+  <si>
+    <t>3Z4S-LE SV-EXR50</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, pro C-montáž, prodlužovací kroužek, 50 mm</t>
+  </si>
+  <si>
+    <t>optika45</t>
+  </si>
+  <si>
+    <t>3Z4S-LE VS-EXR/M42</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, pro M42-montáž, prodlužovací kroužek, sada 5 kroužků (20, 10, 8, 2, 1 mm)</t>
+  </si>
+  <si>
+    <t>optika46</t>
+  </si>
+  <si>
+    <t>3Z4S-LE VS-HVA1226</t>
+  </si>
+  <si>
+    <t>Objektiv, ultra vysoké rozlišení, nízké zkreslení 12 mm pro 1/1" velik</t>
+  </si>
+  <si>
+    <t>optika47</t>
+  </si>
+  <si>
+    <t>3Z4S-LE VS-HVA1626</t>
+  </si>
+  <si>
+    <t>Objektiv, ultra vysoké rozlišení, nízké zkreslení 16 mm pro 1/1" velik</t>
+  </si>
+  <si>
+    <t>optika48</t>
+  </si>
+  <si>
+    <t>3Z4S-LE VS-HVA2524</t>
+  </si>
+  <si>
+    <t>Objektiv, ultra vysoké rozlišení, nízké zkreslení 25 mm pro 1/1" velik</t>
+  </si>
+  <si>
+    <t>optika49</t>
+  </si>
+  <si>
+    <t>3Z4S-LE VS-HVA3522</t>
+  </si>
+  <si>
+    <t>Objektiv, ultra vysoké rozlišení, nízké zkreslení 35 mm pro 1/1" velik</t>
+  </si>
+  <si>
+    <t>optika50</t>
+  </si>
+  <si>
+    <t>3Z4S-LE VS-HVA5024</t>
+  </si>
+  <si>
+    <t>Objektiv, ultra vysoké rozlišení, nízké zkreslení 50 mm pro 1/1" velik</t>
+  </si>
+  <si>
+    <t>optika51</t>
+  </si>
+  <si>
+    <t>3Z4S-LE VS-L10028/M42-10</t>
+  </si>
+  <si>
+    <t>příslušenství pro kamery, čočky, maximální kompatibilní čip CCD 1,8", ohnisková vzdálenost 100 mm, nejmenší vzdálenost 409 mm, světelnost 2,8 až 16, pro montáž M42, revisoin 1</t>
+  </si>
+  <si>
+    <t>optika52</t>
+  </si>
+  <si>
+    <t>3Z4S-LE VS-L1828/M42-10</t>
+  </si>
+  <si>
+    <t>příslušenství pro kamery, čočky, maximální kompatibilní čip CCD 1,8", ohnisková vzdálenost 18 mm, nejmenší vzdálenost 137,9 mm, světelnost 2,8 až 16, pro montáž M42, revisoin 1</t>
+  </si>
+  <si>
+    <t>optika53</t>
+  </si>
+  <si>
+    <t>3Z4S-LE VS-L2526/M42-10</t>
+  </si>
+  <si>
+    <t>příslušenství pro kamery, čočky, maximální kompatibilní čip CCD 1,8", ohnisková vzdálenost 25 mm, nejmenší vzdálenost 198,1 mm, světelnost 2,6 až 16, pro montáž M42, revisoin 1</t>
+  </si>
+  <si>
+    <t>optika54</t>
+  </si>
+  <si>
+    <t>3Z4S-LE VS-L3528/M42-10</t>
+  </si>
+  <si>
+    <t>příslušenství pro kamery, čočky, maximální kompatibilní čip CCD 1,8", ohnisková vzdálenost 35 mm, nejmenší vzdálenost 112,8 mm, světelnost 2,8 až 16, pro montáž M42, revisoin 1</t>
+  </si>
+  <si>
+    <t>optika55</t>
+  </si>
+  <si>
+    <t>3Z4S-LE VS-L5028/M42-10</t>
+  </si>
+  <si>
+    <t>příslušenství pro kamery, čočky, maximální kompatibilní čip CCD 1,8", ohnisková vzdálenost 50 mm, nejmenší vzdálenost 181,4 mm, světelnost 2,8 až 16, pro montáž M42, revisoin 1</t>
+  </si>
+  <si>
+    <t>optika56</t>
+  </si>
+  <si>
+    <t>3Z4S-LE VS-L8540/M42-10</t>
+  </si>
+  <si>
+    <t>příslušenství pro kamery, čočky, maximální kompatibilní čip CCD 1,8", ohnisková vzdálenost 85 mm, nejmenší vzdálenost 285 mm, světelnost 4,0 až 16, pro montáž M42, revisoin 1</t>
+  </si>
+  <si>
+    <t>optika57</t>
+  </si>
+  <si>
+    <t>3Z4S-LE VS-LLD12.5</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, čočky, pro kamery s C-montáží, čočky s ultravysokým rozlišením, pro CCD 4/3", ohnisková vzdálenost 12,5 mm, nejmenší vzdálenost 40,9 mm, světelnost 2,5 až 16</t>
+  </si>
+  <si>
+    <t>optika58</t>
+  </si>
+  <si>
+    <t>3Z4S-LE VS-LLD18</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, čočky, pro kamery s C-montáží, čočky s ultravysokým rozlišením, pro CCD 4/3", ohnisková vzdálenost 18 mm, nejmenší vzdálenost 53,8 mm, světelnost 2,1 až 16</t>
+  </si>
+  <si>
+    <t>optika59</t>
+  </si>
+  <si>
+    <t>3Z4S-LE VS-LLD25</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, čočky, pro kamery s C-montáží, čočky s ultravysokým rozlišením, pro CCD 4/3", ohnisková vzdálenost 25 mm, nejmenší vzdálenost 66 mm, světelnost 2,1 až 16</t>
+  </si>
+  <si>
+    <t>optika60</t>
+  </si>
+  <si>
+    <t>3Z4S-LE VS-LLD35</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, čočky, pro kamery s C-montáží, čočky s ultravysokým rozlišením, pro CCD 4/3", ohnisková vzdálenost 35 mm, nejmenší vzdálenost 129,5 mm, světelnost 2,2 až 16</t>
+  </si>
+  <si>
+    <t>optika61</t>
+  </si>
+  <si>
+    <t>3Z4S-LE VS-LLD50</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, čočky, pro kamery s C-montáží, čočky s ultravysokým rozlišením, pro CCD 4/3", ohnisková vzdálenost 50 mm, nejmenší vzdálenost 205,4 mm, světelnost 2,2 až 16</t>
+  </si>
+  <si>
+    <t>optika62</t>
+  </si>
+  <si>
+    <t>3Z4S-LE VS-MC08H1</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, pro C-montáž, čočky s vysokým rozlišením, odolné vibracím a nárazu, pro kamery s C montáží, ohnisková vzdálenost 8 mm, pro CCD 1", čočka s clonovým systémem</t>
+  </si>
+  <si>
+    <t>optika63</t>
+  </si>
+  <si>
+    <t>3Z4S-LE VS-MC12H1</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, pro C-montáž, čočky s vysokým rozlišením, odolné vibracím a nárazu, pro kamery s C montáží, ohnisková vzdálenost 12 mm, pro CCD 1", čočka s clonovým systémem</t>
+  </si>
+  <si>
+    <t>optika64</t>
+  </si>
+  <si>
+    <t>3Z4S-LE VS-MC16H1</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, pro C-montáž, čočky s vysokým rozlišením, odolné vibracím a nárazu, pro kamery s C montáží, ohnisková vzdálenost 16 mm, pro CCD 1", čočka s clonovým systémem</t>
+  </si>
+  <si>
+    <t>optika65</t>
+  </si>
+  <si>
+    <t>3Z4S-LE VS-MC35H1</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, pro C-montáž, čočky s vysokým rozlišením, odolné vibracím a nárazu, pro kamery s C montáží, ohnisková vzdálenost 35 mm, pro CCD 1" (typ A pro 2/3"), čočka s clonovým systémem</t>
+  </si>
+  <si>
+    <t>optika66</t>
+  </si>
+  <si>
+    <t>3Z4S-LE VS-MC50H1</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, pro C-montáž, čočky s vysokým rozlišením, odolné vibracím a nárazu, pro kamery s C montáží, ohnisková vzdálenost 50 mm, pro CCD 1" (typ A pro2/3"), čočka s clonovým systémem</t>
+  </si>
+  <si>
+    <t>optika67</t>
+  </si>
+  <si>
+    <t>3Z4S-LE VS-MCA10</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, pro C-montáž, čočky odolné nárazu a vibracím, maximální vnější průměr 31 mm, ohnisková vzdálenost 10 mm, pro CCD 1/3", světelnost 2 (pevná)</t>
+  </si>
+  <si>
+    <t>optika68</t>
+  </si>
+  <si>
+    <t>3Z4S-LE VS-MCA10-F5.6</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, pro C-montáž, čočky odolné nárazu a vibracím, maximální vnější průměr 31 mm, ohnisková vzdálenost 10 mm, pro CCD 1/3", světelnost 5,6 (pevná)</t>
+  </si>
+  <si>
+    <t>optika69</t>
+  </si>
+  <si>
+    <t>3Z4S-LE VS-MCA15</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, pro C-montáž, čočky odolné nárazu a vibracím, maximální vnější průměr 31 mm, ohnisková vzdálenost 15 mm, pro CCD 2/3", světelnost 2 (pevná)</t>
+  </si>
+  <si>
+    <t>optika70</t>
+  </si>
+  <si>
+    <t>3Z4S-LE VS-MCA15-F5.6</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, pro C-montáž, čočky odolné nárazu a vibracím, maximální vnější průměr 31 mm, ohnisková vzdálenost 15 mm, pro CCD 2/3", světelnost 5,6 (pevná)</t>
+  </si>
+  <si>
+    <t>optika71</t>
+  </si>
+  <si>
+    <t>3Z4S-LE VS-MCA20</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, pro C-montáž, čočky odolné nárazu a vibracím, maximální vnější průměr 31 mm, ohnisková vzdálenost 20 mm, pro CCD 2/3", světelnost 2 (pevná)</t>
+  </si>
+  <si>
+    <t>optika72</t>
+  </si>
+  <si>
+    <t>3Z4S-LE VS-MCA20-F5.6</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, pro C-montáž, čočky odolné nárazu a vibracím, maximální vnější průměr 31 mm, ohnisková vzdálenost 20 mm, pro CCD 2/3", světelnost 5,6 (pevná)</t>
+  </si>
+  <si>
+    <t>optika73</t>
+  </si>
+  <si>
+    <t>3Z4S-LE VS-MCA25</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, pro C-montáž, čočky odolné nárazu a vibracím, maximální vnější průměr 31 mm, ohnisková vzdálenost 25 mm, pro CCD 1" (typ A pro 2/3"), světelnost 2 (pevná)</t>
+  </si>
+  <si>
+    <t>optika74</t>
+  </si>
+  <si>
+    <t>3Z4S-LE VS-MCA25-F5.6</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, pro C-montáž, čočky odolné nárazu a vibracím, maximální vnější průměr 31 mm, ohnisková vzdálenost 25 mm, pro CCD 1" (typ A pro 2/3"), světelnost 5,6 (pevná)</t>
+  </si>
+  <si>
+    <t>optika75</t>
+  </si>
+  <si>
+    <t>3Z4S-LE VS-MCA30</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, pro C-montáž, čočky odolné nárazu a vibracím, maximální vnější průměr 31 mm, ohnisková vzdálenost 30 mm, pro CCD 2/3", světelnost 2 (pevná)</t>
+  </si>
+  <si>
+    <t>optika76</t>
+  </si>
+  <si>
+    <t>3Z4S-LE VS-MCA30-F5.6</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, pro C-montáž, čočky odolné nárazu a vibracím, maximální vnější průměr 31 mm, ohnisková vzdálenost 30 mm, pro CCD 2/3", světelnost 5,6 (pevná)</t>
+  </si>
+  <si>
+    <t>optika77</t>
+  </si>
+  <si>
+    <t>3Z4S-LE VS-MCA30-F8</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, pro C-montáž, čočky odolné nárazu a vibracím, maximální vnější průměr 31 mm, ohnisková vzdálenost 30 mm, pro CCD 2/3", světelnost 8 (pevná)</t>
+  </si>
+  <si>
+    <t>optika78</t>
+  </si>
+  <si>
+    <t>3Z4S-LE VS-MCA35</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, pro C-montáž, čočky odolné nárazu a vibracím, maximální vnější průměr 31 mm, ohnisková vzdálenost 35 mm, pro CCD 1" (typ A pro 2/3"), světelnost 2 (pevná)</t>
+  </si>
+  <si>
+    <t>optika79</t>
+  </si>
+  <si>
+    <t>3Z4S-LE VS-MCA35-F5.6</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, pro C-montáž, čočky odolné nárazu a vibracím, maximální vnější průměr 31 mm, ohnisková vzdálenost 35 mm, pro CCD 1" (typ A pro 2/3"), světelnost 5,6 (pevná),</t>
+  </si>
+  <si>
+    <t>optika80</t>
+  </si>
+  <si>
+    <t>3Z4S-LE VS-MCA4</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, pro C-montáž, čočky odolné nárazu a vibracím, maximální vnější průměr 31 mm, ohnisková vzdálenost 4 mm, pro CCD 1/3", světelnost 2 (pevná)</t>
+  </si>
+  <si>
+    <t>optika81</t>
+  </si>
+  <si>
+    <t>3Z4S-LE VS-MCA50</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, pro C-montáž, čočky odolné nárazu a vibracím, maximální vnější průměr 31 mm, ohnisková vzdálenost 50 mm, pro CCD 1" (typ A pro2/3"), světelnost 2 (pevná)</t>
+  </si>
+  <si>
+    <t>optika82</t>
+  </si>
+  <si>
+    <t>3Z4S-LE VS-MCA50-F5.6</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, pro C-montáž, čočky odolné nárazu a vibracím, maximální vnější průměr 31 mm, ohnisková vzdálenost 50 mm, pro CCD 1" (typ A pro2/3"), světelnost 5,6 (pevná)</t>
+  </si>
+  <si>
+    <t>optika83</t>
+  </si>
+  <si>
+    <t>3Z4S-LE VS-MCA6.5</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, pro C-montáž, čočky odolné nárazu a vibracím, maximální vnější průměr 31 mm, ohnisková vzdálenost 6,5 mm, pro CCD 1/3", světelnost 2 (pevná)</t>
+  </si>
+  <si>
+    <t>optika84</t>
+  </si>
+  <si>
+    <t>3Z4S-LE VS-MCA6.5-F5.6</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, pro C-montáž, čočky odolné nárazu a vibracím, maximální vnější průměr 31 mm, ohnisková vzdálenost 6,5 mm, pro CCD 1/3", světelnost 5,6 (pevná)</t>
+  </si>
+  <si>
+    <t>optika85</t>
+  </si>
+  <si>
+    <t>3Z4S-LE VS-MCA75</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, pro C-montáž, čočky odolné nárazu a vibracím, maximální vnější průměr 31 mm, ohnisková vzdálenost 75 mm, pro CCD 2/3", světelnost 2 (pevná)</t>
+  </si>
+  <si>
+    <t>optika86</t>
+  </si>
+  <si>
+    <t>3Z4S-LE VS-MCA75-F5.6</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, pro C-montáž, čočky odolné nárazu a vibracím, maximální vnější průměr 31 mm, ohnisková vzdálenost 75 mm, pro CCD 2/3", světelnost 5,6 (pevná)</t>
+  </si>
+  <si>
+    <t>optika87</t>
+  </si>
+  <si>
+    <t>3Z4S-LE VS-MCA75-F8</t>
+  </si>
+  <si>
+    <t>Příslušenství pro kamery, pro C-montáž, čočky odolné nárazu a vibracím, maximální vnější průměr 31 mm, ohnisková vzdálenost 75 mm, pro CCD 2/3", světelnost 8 (pevná),</t>
+  </si>
+  <si>
+    <t>optika88</t>
   </si>
   <si>
     <t xml:space="preserve">Keyence XG-X 
@@ -404,16 +1167,167 @@
     <t>FH-SMX12-PL</t>
   </si>
   <si>
+    <t>FZ-VS3 10M</t>
+  </si>
+  <si>
+    <t>příslušenství kamerových systémů, FH a FZ, kabel ke standardní kameře, 10m http://industrial.omron.eu/en/search?q=G639</t>
+  </si>
+  <si>
+    <t>FZ-VS3 2M</t>
+  </si>
+  <si>
+    <t>příslušenství kamerových systémů, FH a FZ, kabel ke standardní kameře, 2m
+http://industrial.omron.co.uk/en/search?q=G639</t>
+  </si>
+  <si>
+    <t>FZ-VS3 3M</t>
+  </si>
+  <si>
+    <t>příslušenství kamerových systémů, FH a FZ, kabel ke standardní kameře, 3m
+http://industrial.omron.co.uk/en/search?q=G639</t>
+  </si>
+  <si>
+    <t>FZ-VS3 5M</t>
+  </si>
+  <si>
+    <t>příslušenství kamerových systémů, FH a FZ, kabel ke standardní kameře, 5m
+http://industrial.omron.eu/en/search?q=G639</t>
+  </si>
+  <si>
+    <t>FZ-VS4 15M</t>
+  </si>
+  <si>
+    <t>příslušenství kamerových systémů, FH a FZ, kabel pro kameru, velký dosah, 15m
+http://industrial.omron.co.uk/en/search?q=G639</t>
+  </si>
+  <si>
+    <t>FZ-VSB3 10M</t>
+  </si>
+  <si>
+    <t>příslušenství kamerových systémů, FH a FZ, kabel pro kameru, odolný ohybu, 10m
+http://industrial.omron.co.uk/en/search?q=G639</t>
+  </si>
+  <si>
+    <t>FZ-VSB3 5M</t>
+  </si>
+  <si>
+    <t>příslušenství kamerových systémů, FH a FZ, kabel pro kameru, odolný ohybu, 5m, revize 1</t>
+  </si>
+  <si>
+    <t>FZ-VSBX 10M</t>
+  </si>
+  <si>
+    <t>Ultra bend resistant camera cable, 10 m</t>
+  </si>
+  <si>
+    <t>FZ-VSBX 5M</t>
+  </si>
+  <si>
+    <t>Ultra bend resistant camera cable, 5 m</t>
+  </si>
+  <si>
+    <t>FZ-VSL3 10M</t>
+  </si>
+  <si>
+    <t>příslušenství kamerových systémů, FH a FZ, kabel pro kameru, standardní, konektor úhlový, 10m
+http://industrial.omron.co.uk/en/search?q=G639</t>
+  </si>
+  <si>
+    <t>FZ-VSL3 2M</t>
+  </si>
+  <si>
+    <t>příslušenství kamerových systémů, FH a FZ, kabel pro kameru, standardní, konektor úhlový, 2m
+http://industrial.omron.eu/en/search?q=G639</t>
+  </si>
+  <si>
+    <t>FZ-VSL3 3M</t>
+  </si>
+  <si>
+    <t>příslušenství kamerových systémů, FH a FZ, kabel pro kameru, standardní, konektor úhlový, 3m
+http://industrial.omron.co.uk/en/search?q=G639</t>
+  </si>
+  <si>
+    <t>FZ-VSL3 5M</t>
+  </si>
+  <si>
+    <t>příslušenství kamerových systémů, FH a FZ, kabel pro kameru, standardní, konektor úhlový, 5m
+http://industrial.omron.eu/en/search?q=G639</t>
+  </si>
+  <si>
+    <t>FZ-VSL4 15M</t>
+  </si>
+  <si>
+    <t>příslušenství kamerových systémů, FH a FZ, kabel pro kameru, standardní, konektor úhlový, 15m
+http://industrial.omron.co.uk/en/search?q=G639</t>
+  </si>
+  <si>
+    <t>FZ-VSLB3 10M</t>
+  </si>
+  <si>
+    <t>příslušenství kamerových systémů, FH a FZ, kabel pro kameru, odolný ohybu, konektor úhlový, 10m
+http://industrial.omron.co.uk/en/search?q=G639</t>
+  </si>
+  <si>
+    <t>FZ-VSLB3 2M</t>
+  </si>
+  <si>
+    <t>příslušenství kamerových systémů, FH a FZ, kabel pro kameru, odolný ohybu, konektor úhlový, 2m
+http://industrial.omron.co.uk/en/search?q=G639</t>
+  </si>
+  <si>
+    <t>FZ-VSLB3 3M</t>
+  </si>
+  <si>
+    <t>příslušenství kamerových systémů, FH a FZ, kabel pro kameru, odolný ohybu, konektor úhlový, 3m
+http://industrial.omron.co.uk/en/search?q=G639</t>
+  </si>
+  <si>
+    <t>FZ-VSLB3 5M</t>
+  </si>
+  <si>
+    <t>příslušenství kamerových systémů, FH a FZ, kabel pro kameru, odolný ohybu, konektor úhlový, 5m</t>
+  </si>
+  <si>
+    <t>rozšíření kontroleru</t>
+  </si>
+  <si>
+    <t>SD karta</t>
+  </si>
+  <si>
+    <t>monitor</t>
+  </si>
+  <si>
+    <t>HDD</t>
+  </si>
+  <si>
+    <t>konzole</t>
+  </si>
+  <si>
+    <t>NAS</t>
+  </si>
+  <si>
+    <t>kamera</t>
+  </si>
+  <si>
+    <t>kabel ke kameře</t>
+  </si>
+  <si>
+    <t>FH-MT12</t>
+  </si>
+  <si>
+    <t>dotyková obrazovka kamerového systému FH 12"</t>
+  </si>
+  <si>
     <t>CA-E100</t>
   </si>
   <si>
     <t>Area camera input unit</t>
   </si>
   <si>
-    <t>FH-MT12</t>
-  </si>
-  <si>
-    <t>dotyková obrazovka kamerového systému FH 12"</t>
+    <t>FH-SM-XLC</t>
+  </si>
+  <si>
+    <t>montážní úchyt kamery FH pro FH-SM</t>
   </si>
   <si>
     <t>CA-E200</t>
@@ -422,12 +1336,6 @@
     <t>High-resolution area camera input unit</t>
   </si>
   <si>
-    <t>FH-SM-XLC</t>
-  </si>
-  <si>
-    <t>montážní úchyt kamery FH pro FH-SM</t>
-  </si>
-  <si>
     <t>CA-E100L</t>
   </si>
   <si>
@@ -492,49 +1400,13 @@
   </si>
   <si>
     <t>EtherNet/IP module</t>
-  </si>
-  <si>
-    <t>optika1</t>
-  </si>
-  <si>
-    <t>optika2</t>
-  </si>
-  <si>
-    <t>optika3</t>
-  </si>
-  <si>
-    <t>optika4</t>
-  </si>
-  <si>
-    <t>optika5</t>
-  </si>
-  <si>
-    <t>optika6</t>
-  </si>
-  <si>
-    <t>optika7</t>
-  </si>
-  <si>
-    <t>optika8</t>
-  </si>
-  <si>
-    <t>optika9</t>
-  </si>
-  <si>
-    <t>optika10</t>
-  </si>
-  <si>
-    <t>optika11</t>
-  </si>
-  <si>
-    <t>FH-Lite controller, standard grade, box type, 4 camera, , W10 IoT Ente</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -554,6 +1426,15 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="2">
@@ -604,7 +1485,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -625,23 +1506,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -924,11 +1812,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.42578125" customWidth="1"/>
     <col min="2" max="2" width="81.28515625" customWidth="1"/>
@@ -936,278 +1824,278 @@
     <col min="4" max="4" width="55.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="8" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="9"/>
+      <c r="D1" s="16"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="B6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="B7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="D7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="C8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="4" t="s">
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="D9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="B10" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="B11" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="C11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="4" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="4" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="4" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="4" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C16" s="1"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="4" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C17" s="1"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="4" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C18" s="1"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="4" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C19" s="1"/>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="4" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C20" s="1"/>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="4" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C21" s="1"/>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="4" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C22" s="1"/>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" s="4" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>167</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1221,110 +2109,978 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6243DA3-0875-4C03-8E69-F223C9363894}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="24.140625" customWidth="1"/>
+    <col min="2" max="2" width="82" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="8" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="9"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="D1" s="16"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C18" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C20" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C21" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C22" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C23" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C24" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C25" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C26" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C27" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="C28" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="C29" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C30" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="C31" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="8"/>
+      <c r="B32" s="8"/>
+      <c r="C32" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="C33" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="C34" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="C35" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="C36" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="C37" t="s">
         <v>156</v>
       </c>
-      <c r="C2" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="C3" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B38" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="C4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C38" t="s">
         <v>159</v>
       </c>
-      <c r="C5" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="C6" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B39" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="C7" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="C39" t="s">
         <v>162</v>
       </c>
-      <c r="C8" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="C9" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B40" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="C10" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="C40" t="s">
         <v>165</v>
       </c>
-      <c r="C11" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="C12" t="s">
-        <v>166</v>
+      <c r="B41" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="C41" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="C42" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C43" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C44" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C45" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="C46" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C47" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="C48" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="C49" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="C50" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="C51" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="C52" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="C53" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="C54" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="C55" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="C56" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="C57" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="C58" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="C59" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="C60" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="C61" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="C62" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="C63" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="C64" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="C65" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="C66" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="C67" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="C68" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="C69" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="C70" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="B71" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="C71" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="B72" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="C72" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="B73" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="C73" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="B74" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="C74" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="B75" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="C75" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="C76" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="B77" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="C77" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="B78" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="C78" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="C79" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="B80" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="C80" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="B81" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="C81" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="B82" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="C82" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="B83" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="C83" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="B84" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="C84" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="B85" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="C85" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" s="8" t="s">
+        <v>301</v>
+      </c>
+      <c r="B86" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="C86" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="B87" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="C87" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="B88" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="C88" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="B89" s="8" t="s">
+        <v>311</v>
+      </c>
+      <c r="C89" t="s">
+        <v>312</v>
       </c>
     </row>
   </sheetData>
@@ -1339,306 +3095,450 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="81.42578125" customWidth="1"/>
+    <col min="2" max="2" width="150.5703125" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="D1" s="12"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" s="17"/>
+      <c r="C1" s="13" t="s">
+        <v>313</v>
+      </c>
+      <c r="D1" s="17"/>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>314</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>315</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>67</v>
+        <v>316</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>67</v>
+        <v>316</v>
       </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>317</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>69</v>
+        <v>318</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>70</v>
+        <v>319</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>70</v>
+        <v>319</v>
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>320</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>321</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>73</v>
+        <v>322</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>73</v>
+        <v>322</v>
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>323</v>
       </c>
       <c r="B5" t="s">
-        <v>75</v>
+        <v>324</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>76</v>
+        <v>325</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>76</v>
+        <v>325</v>
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>326</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>78</v>
+        <v>327</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>79</v>
+        <v>328</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>79</v>
+        <v>328</v>
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>80</v>
+        <v>329</v>
       </c>
       <c r="B7" t="s">
-        <v>81</v>
+        <v>330</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>82</v>
+        <v>331</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>82</v>
+        <v>331</v>
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>83</v>
+        <v>332</v>
       </c>
       <c r="B8" t="s">
-        <v>84</v>
+        <v>333</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>85</v>
+        <v>334</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>85</v>
+        <v>334</v>
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>86</v>
+        <v>335</v>
       </c>
       <c r="B9" t="s">
-        <v>87</v>
+        <v>336</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>88</v>
+        <v>337</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>88</v>
+        <v>337</v>
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>89</v>
+        <v>338</v>
       </c>
       <c r="B10" t="s">
-        <v>90</v>
+        <v>339</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>91</v>
+        <v>340</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>91</v>
+        <v>340</v>
       </c>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>92</v>
+        <v>341</v>
       </c>
       <c r="B11" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>94</v>
+        <v>343</v>
       </c>
       <c r="B12" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>96</v>
+        <v>345</v>
       </c>
       <c r="B13" t="s">
-        <v>97</v>
+        <v>346</v>
       </c>
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>98</v>
+        <v>347</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>100</v>
+        <v>349</v>
       </c>
       <c r="B15" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>102</v>
+        <v>351</v>
       </c>
       <c r="B16" t="s">
-        <v>103</v>
+        <v>352</v>
       </c>
       <c r="C16" s="5"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>104</v>
+        <v>353</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>106</v>
+        <v>355</v>
       </c>
       <c r="B18" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>108</v>
+        <v>357</v>
       </c>
       <c r="B19" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>110</v>
+        <v>359</v>
       </c>
       <c r="B20" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>112</v>
+        <v>361</v>
       </c>
       <c r="B21" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>114</v>
+        <v>363</v>
       </c>
       <c r="B22" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>116</v>
+        <v>365</v>
       </c>
       <c r="B23" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>118</v>
+        <v>367</v>
       </c>
       <c r="B24" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>120</v>
+        <v>369</v>
       </c>
       <c r="B25" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>122</v>
+        <v>371</v>
       </c>
       <c r="B26" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>122</v>
+        <v>371</v>
       </c>
       <c r="B27" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>125</v>
+        <v>374</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="8" t="s">
+        <v>375</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="8" t="s">
+        <v>377</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="8" t="s">
+        <v>383</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="8" t="s">
+        <v>385</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="8" t="s">
+        <v>387</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="8" t="s">
+        <v>389</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="8" t="s">
+        <v>391</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="8" t="s">
+        <v>393</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="8" t="s">
+        <v>395</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="8" t="s">
+        <v>397</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="8" t="s">
+        <v>399</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="8" t="s">
+        <v>401</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="8" t="s">
+        <v>403</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="8" t="s">
+        <v>407</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="8" t="s">
+        <v>409</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>410</v>
       </c>
     </row>
   </sheetData>
@@ -1655,10 +3555,10 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.5703125" customWidth="1"/>
     <col min="2" max="2" width="40.5703125" customWidth="1"/>
@@ -1666,230 +3566,230 @@
     <col min="4" max="4" width="46.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:5" ht="15" customHeight="1">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="13" t="s">
+      <c r="B1" s="17"/>
+      <c r="C1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="12"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D1" s="17"/>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="6" t="s">
-        <v>2</v>
+        <v>411</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6" t="s">
-        <v>2</v>
+        <v>411</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>412</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>3</v>
+        <v>412</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>413</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>4</v>
+        <v>413</v>
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>414</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>5</v>
+        <v>414</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>415</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>6</v>
+        <v>415</v>
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>416</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>7</v>
+        <v>416</v>
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>417</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>8</v>
+        <v>417</v>
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>418</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>9</v>
+        <v>418</v>
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>128</v>
+        <v>419</v>
       </c>
       <c r="B10" t="s">
-        <v>129</v>
+        <v>420</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>126</v>
+        <v>421</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>132</v>
+        <v>423</v>
       </c>
       <c r="B11" t="s">
-        <v>133</v>
+        <v>424</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>130</v>
+        <v>425</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="C12" s="6" t="s">
-        <v>134</v>
+        <v>427</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="C13" s="6" t="s">
-        <v>136</v>
+        <v>429</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="C14" s="6" t="s">
-        <v>138</v>
+        <v>431</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="C15" s="6" t="s">
-        <v>140</v>
+        <v>433</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="C16" s="6" t="s">
-        <v>142</v>
+        <v>435</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4">
       <c r="C17" s="6" t="s">
-        <v>144</v>
+        <v>437</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4">
       <c r="C18" s="6" t="s">
-        <v>146</v>
+        <v>439</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4">
       <c r="C19" s="1" t="s">
-        <v>148</v>
+        <v>441</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4">
       <c r="C20" s="1" t="s">
-        <v>150</v>
+        <v>443</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4">
       <c r="C21" s="1" t="s">
-        <v>152</v>
+        <v>445</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4">
       <c r="C22" s="1" t="s">
-        <v>154</v>
+        <v>447</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="28" spans="3:4">
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:4">
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:4">
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:4">
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:4">
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:3">
       <c r="C33" s="1"/>
     </row>
   </sheetData>
@@ -1899,4 +3799,265 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="f1000b3d-15af-42f4-8b30-1751694c7388" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0a44024f-7437-4220-82e3-7a609f3cc5d0">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100AC30A1654071464B83845798603538A6" ma:contentTypeVersion="14" ma:contentTypeDescription="Vytvoří nový dokument" ma:contentTypeScope="" ma:versionID="9168d1d45adf597786ba4404c21a0f63">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f1000b3d-15af-42f4-8b30-1751694c7388" xmlns:ns3="0a44024f-7437-4220-82e3-7a609f3cc5d0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2a603704bc0fe2974ac9a36df3b95205" ns2:_="" ns3:_="">
+    <xsd:import namespace="f1000b3d-15af-42f4-8b30-1751694c7388"/>
+    <xsd:import namespace="0a44024f-7437-4220-82e3-7a609f3cc5d0"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns2:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns3:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns2:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceSearchProperties" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="f1000b3d-15af-42f4-8b30-1751694c7388" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="8" nillable="true" ma:displayName="Sdílí se s" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="9" nillable="true" ma:displayName="Sdílené s podrobnostmi" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="17" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{26d47648-00f3-4c5f-bb64-a2adc96c09eb}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="f1000b3d-15af-42f4-8b30-1751694c7388">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="0a44024f-7437-4220-82e3-7a609f3cc5d0" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="10" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="11" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="12" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="13" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="14" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="16" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Značky obrázků" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="8f46599a-a670-45bb-b2ce-f3c9690acef5" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="18" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="19" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="20" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="21" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Typ obsahu"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Nadpis"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB475825-C6B0-46AE-A469-0210B2AABFAD}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20F53162-DA3D-49C7-BB54-6E566081E5DD}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4401364-4573-4AA3-A01C-3A51337634B0}"/>
 </file>
</xml_diff>

<commit_message>
přepínání mezi výrobci, scroll menu upgrade, podbarvení kontrolerů...
</commit_message>
<xml_diff>
--- a/catalogue_manager/Sharepoint_databaze.xlsx
+++ b/catalogue_manager/Sharepoint_databaze.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakub.hlavacek.local\Desktop\JHV\Work\catalogue_manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{5854EDA4-EDB7-4482-88EE-7784F287C2DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E993AD4-A753-48D1-8614-FC36D62435F8}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="13_ncr:1_{5854EDA4-EDB7-4482-88EE-7784F287C2DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0FDF745-B05A-43DC-A82C-1358DC1737DF}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kontrolery" sheetId="2" r:id="rId1"/>
     <sheet name="Optika" sheetId="6" r:id="rId2"/>
     <sheet name="Kamery" sheetId="3" r:id="rId3"/>
-    <sheet name="Přislušenství" sheetId="4" r:id="rId4"/>
+    <sheet name="Kabely" sheetId="7" r:id="rId4"/>
+    <sheet name="Přislušenství" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="450">
   <si>
     <t>Omron FZ/FH</t>
   </si>
@@ -287,6 +288,9 @@
     <t>optika9</t>
   </si>
   <si>
+    <t>***</t>
+  </si>
+  <si>
     <t>optika10</t>
   </si>
   <si>
@@ -980,8 +984,7 @@
     <t>optika88</t>
   </si>
   <si>
-    <t xml:space="preserve">Keyence XG-X 
-</t>
+    <t xml:space="preserve">Keyence XG-X </t>
   </si>
   <si>
     <t>FH-SC</t>
@@ -1406,7 +1409,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1435,6 +1438,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="238"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1485,7 +1494,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1520,6 +1529,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1828,11 +1840,11 @@
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
+      <c r="B1" s="17"/>
       <c r="C1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="16"/>
+      <c r="D1" s="17"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5">
@@ -2111,7 +2123,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6243DA3-0875-4C03-8E69-F223C9363894}">
   <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A41" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -2125,11 +2137,11 @@
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
+      <c r="B1" s="17"/>
       <c r="C1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="16"/>
+      <c r="D1" s="17"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="8"/>
@@ -2227,860 +2239,866 @@
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="8"/>
+      <c r="A11" s="8" t="s">
+        <v>82</v>
+      </c>
       <c r="B11" s="8"/>
       <c r="C11" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C12" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C13" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C14" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C15" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="8" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C16" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C17" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="8" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C18" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="8"/>
+      <c r="A19" s="8" t="s">
+        <v>82</v>
+      </c>
       <c r="B19" s="8"/>
       <c r="C19" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="8" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C20" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C21" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="8" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C22" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C23" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="8" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C24" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="8" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C25" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="8" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C26" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="8" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C27" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="8" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C28" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="8" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C29" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="8" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C30" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="8" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C31" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="8"/>
+      <c r="A32" s="8" t="s">
+        <v>82</v>
+      </c>
       <c r="B32" s="8"/>
       <c r="C32" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="8" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C33" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="8" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C34" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="8" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C35" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C36" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C37" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="8" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C38" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="8" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C39" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="8" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C40" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C41" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="8" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C42" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="8" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C43" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="8" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C44" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="8" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C45" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="8" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C46" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C47" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="8" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C48" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="8" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C49" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="8" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C50" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="8" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C51" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="8" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C52" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="8" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C53" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="8" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C54" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="8" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C55" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="8" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C56" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="8" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C57" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="8" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C58" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="8" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C59" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="8" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C60" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="8" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C61" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="8" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C62" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="8" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C63" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="8" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C64" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" s="8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C65" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="8" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C66" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="8" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C67" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="8" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C68" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="8" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C69" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" s="8" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C70" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" s="8" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C71" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" s="8" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C72" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" s="8" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C73" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" s="8" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C74" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" s="8" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C75" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" s="8" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C76" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" s="8" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C77" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" s="8" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C78" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" s="8" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C79" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" s="8" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C80" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" s="8" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C81" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" s="8" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C82" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" s="8" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C83" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" s="8" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C84" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" s="8" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C85" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" s="8" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C86" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" s="8" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C87" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" s="8" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C88" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" s="8" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C89" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
   </sheetData>
@@ -3095,10 +3113,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3113,280 +3131,277 @@
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
+      <c r="B1" s="18"/>
       <c r="C1" s="13" t="s">
-        <v>313</v>
-      </c>
-      <c r="D1" s="17"/>
+        <v>314</v>
+      </c>
+      <c r="D1" s="18"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B4" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B5" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B7" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B8" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B9" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B10" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B11" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B12" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B13" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C13" s="5"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>347</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>348</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
+        <v>348</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>349</v>
-      </c>
-      <c r="B15" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
+        <v>350</v>
+      </c>
+      <c r="B16" t="s">
         <v>351</v>
-      </c>
-      <c r="B16" t="s">
-        <v>352</v>
       </c>
       <c r="C16" s="5"/>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
+        <v>352</v>
+      </c>
+      <c r="B17" t="s">
         <v>353</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
+        <v>354</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>355</v>
-      </c>
-      <c r="B18" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
+        <v>356</v>
+      </c>
+      <c r="B19" t="s">
         <v>357</v>
-      </c>
-      <c r="B19" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
+        <v>358</v>
+      </c>
+      <c r="B20" t="s">
         <v>359</v>
-      </c>
-      <c r="B20" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
+        <v>360</v>
+      </c>
+      <c r="B21" t="s">
         <v>361</v>
-      </c>
-      <c r="B21" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
+        <v>362</v>
+      </c>
+      <c r="B22" t="s">
         <v>363</v>
-      </c>
-      <c r="B22" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
+        <v>364</v>
+      </c>
+      <c r="B23" t="s">
         <v>365</v>
-      </c>
-      <c r="B23" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
+        <v>366</v>
+      </c>
+      <c r="B24" t="s">
         <v>367</v>
-      </c>
-      <c r="B24" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
+        <v>368</v>
+      </c>
+      <c r="B25" t="s">
         <v>369</v>
-      </c>
-      <c r="B25" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
+        <v>370</v>
+      </c>
+      <c r="B26" t="s">
         <v>371</v>
-      </c>
-      <c r="B26" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B27" t="s">
         <v>373</v>
@@ -3394,151 +3409,15 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
+        <v>372</v>
+      </c>
+      <c r="B28" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="8" t="s">
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
         <v>375</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="8" t="s">
-        <v>377</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="8" t="s">
-        <v>379</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="8" t="s">
-        <v>383</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="8" t="s">
-        <v>385</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="8" t="s">
-        <v>387</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="8" t="s">
-        <v>389</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="8" t="s">
-        <v>391</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
-      <c r="A39" s="8" t="s">
-        <v>393</v>
-      </c>
-      <c r="B39" s="10" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
-      <c r="A40" s="8" t="s">
-        <v>395</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
-      <c r="A41" s="8" t="s">
-        <v>397</v>
-      </c>
-      <c r="B41" s="9" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
-      <c r="A42" s="8" t="s">
-        <v>399</v>
-      </c>
-      <c r="B42" s="10" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
-      <c r="A43" s="8" t="s">
-        <v>401</v>
-      </c>
-      <c r="B43" s="10" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
-      <c r="A44" s="8" t="s">
-        <v>403</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
-      <c r="A45" s="8" t="s">
-        <v>405</v>
-      </c>
-      <c r="B45" s="9" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
-      <c r="A46" s="8" t="s">
-        <v>407</v>
-      </c>
-      <c r="B46" s="9" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2">
-      <c r="A47" s="8" t="s">
-        <v>409</v>
-      </c>
-      <c r="B47" s="9" t="s">
-        <v>410</v>
       </c>
     </row>
   </sheetData>
@@ -3551,11 +3430,188 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04F3B6E1-C926-490E-B179-CA4119029E15}">
+  <dimension ref="A1:D19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="134.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="14" t="s">
+        <v>314</v>
+      </c>
+      <c r="D1" s="14"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="8" t="s">
+        <v>376</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="8" t="s">
+        <v>384</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="8" t="s">
+        <v>390</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="8" t="s">
+        <v>392</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="8" t="s">
+        <v>394</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="8" t="s">
+        <v>398</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="8" t="s">
+        <v>402</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="8" t="s">
+        <v>404</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="8" t="s">
+        <v>406</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="8" t="s">
+        <v>408</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="8" t="s">
+        <v>410</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>411</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3567,211 +3623,211 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="14" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="17"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="6" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="B10" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="B11" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="C12" s="6" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="C13" s="6" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="C14" s="6" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="C15" s="6" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="C16" s="6" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="17" spans="3:4">
       <c r="C17" s="6" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="18" spans="3:4">
       <c r="C18" s="6" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="19" spans="3:4">
       <c r="C19" s="1" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="20" spans="3:4">
       <c r="C20" s="1" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="21" spans="3:4">
       <c r="C21" s="1" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="22" spans="3:4">
       <c r="C22" s="1" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row r="28" spans="3:4">

</xml_diff>

<commit_message>
nový explorer při hledání souboru, None při nahrání programu, import poznámek všude, oprava initial_prefill
</commit_message>
<xml_diff>
--- a/catalogue_manager/Sharepoint_databaze.xlsx
+++ b/catalogue_manager/Sharepoint_databaze.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakub.hlavacek.local\Desktop\JHV\Work\catalogue_manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="13_ncr:1_{5854EDA4-EDB7-4482-88EE-7784F287C2DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0FDF745-B05A-43DC-A82C-1358DC1737DF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{999F4B56-2D42-40C9-8BE9-B468CDF41444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3420" yWindow="3420" windowWidth="28800" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kontrolery" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="449">
   <si>
     <t>Omron FZ/FH</t>
   </si>
@@ -148,9 +148,6 @@
   </si>
   <si>
     <t>FH-5051-10</t>
-  </si>
-  <si>
-    <t>FH vysokorychlostní / vysoce výkonný regulátor, 4 jádra, NPN/PNP, 4 ka</t>
   </si>
   <si>
     <t>FH-5051-20</t>
@@ -1409,7 +1406,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1525,12 +1522,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1540,8 +1539,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1824,11 +1821,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.42578125" customWidth="1"/>
     <col min="2" max="2" width="81.28515625" customWidth="1"/>
@@ -1836,18 +1833,18 @@
     <col min="4" max="4" width="55.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
+      <c r="B1" s="12"/>
       <c r="C1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="17"/>
+      <c r="D1" s="12"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -1862,7 +1859,7 @@
       </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1877,7 +1874,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
@@ -1892,7 +1889,7 @@
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
@@ -1907,7 +1904,7 @@
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
@@ -1922,7 +1919,7 @@
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>20</v>
       </c>
@@ -1937,7 +1934,7 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>23</v>
       </c>
@@ -1952,7 +1949,7 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>26</v>
       </c>
@@ -1967,7 +1964,7 @@
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>30</v>
       </c>
@@ -1982,7 +1979,7 @@
       </c>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>33</v>
       </c>
@@ -1992,122 +1989,118 @@
       <c r="C11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>36</v>
-      </c>
+      <c r="B12" s="4"/>
       <c r="C12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>38</v>
       </c>
       <c r="C13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="C14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="C15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>44</v>
       </c>
       <c r="C16" s="1"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>46</v>
       </c>
       <c r="C17" s="1"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" s="4" t="s">
         <v>46</v>
       </c>
+      <c r="B18" s="4"/>
       <c r="C18" s="1"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C19" s="1"/>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>50</v>
       </c>
       <c r="C20" s="1"/>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>52</v>
       </c>
       <c r="C21" s="1"/>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>54</v>
       </c>
       <c r="C22" s="1"/>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -2123,982 +2116,982 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6243DA3-0875-4C03-8E69-F223C9363894}">
   <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.140625" customWidth="1"/>
     <col min="2" max="2" width="82" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
+      <c r="B1" s="12"/>
       <c r="C1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="17"/>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="D1" s="12"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="8" t="s">
+      <c r="B3" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="C3" t="s">
         <v>59</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="8" t="s">
+      <c r="B4" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="C4" t="s">
         <v>62</v>
       </c>
-      <c r="C4" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="8" t="s">
+      <c r="B5" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="C5" t="s">
         <v>65</v>
       </c>
-      <c r="C5" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="8" t="s">
+      <c r="B6" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="C6" t="s">
         <v>68</v>
       </c>
-      <c r="C6" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="8" t="s">
+      <c r="B7" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="C7" t="s">
         <v>71</v>
       </c>
-      <c r="C7" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="8" t="s">
+      <c r="B8" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="C8" t="s">
         <v>74</v>
       </c>
-      <c r="C8" t="s">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="8" t="s">
+      <c r="B9" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="C9" t="s">
         <v>77</v>
       </c>
-      <c r="C9" t="s">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="8" t="s">
+      <c r="B10" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="C10" t="s">
         <v>80</v>
       </c>
-      <c r="C10" t="s">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="8" t="s">
-        <v>82</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="8" t="s">
+      <c r="B12" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="C12" t="s">
         <v>85</v>
       </c>
-      <c r="C12" t="s">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="8" t="s">
+      <c r="B13" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="C13" t="s">
         <v>88</v>
       </c>
-      <c r="C13" t="s">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="8" t="s">
+      <c r="B14" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="C14" t="s">
         <v>91</v>
       </c>
-      <c r="C14" t="s">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="8" t="s">
+      <c r="B15" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="C15" t="s">
         <v>94</v>
       </c>
-      <c r="C15" t="s">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="8" t="s">
+      <c r="B16" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="C16" t="s">
         <v>97</v>
       </c>
-      <c r="C16" t="s">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="8" t="s">
+      <c r="B17" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="C17" t="s">
         <v>100</v>
       </c>
-      <c r="C17" t="s">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="8" t="s">
+      <c r="B18" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="C18" t="s">
         <v>103</v>
       </c>
-      <c r="C18" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="8" t="s">
+      <c r="B20" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="C20" t="s">
         <v>107</v>
       </c>
-      <c r="C20" t="s">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="8" t="s">
+      <c r="B21" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="C21" t="s">
         <v>110</v>
       </c>
-      <c r="C21" t="s">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="8" t="s">
+      <c r="B22" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="C22" t="s">
         <v>113</v>
       </c>
-      <c r="C22" t="s">
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="8" t="s">
+      <c r="B23" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="C23" t="s">
         <v>116</v>
       </c>
-      <c r="C23" t="s">
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="8" t="s">
+      <c r="B24" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="C24" t="s">
         <v>119</v>
       </c>
-      <c r="C24" t="s">
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="8" t="s">
+      <c r="B25" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="C25" t="s">
         <v>122</v>
       </c>
-      <c r="C25" t="s">
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="8" t="s">
+      <c r="B26" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="C26" t="s">
         <v>125</v>
       </c>
-      <c r="C26" t="s">
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="8" t="s">
+      <c r="B27" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="C27" t="s">
         <v>128</v>
       </c>
-      <c r="C27" t="s">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="8" t="s">
+      <c r="B28" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="C28" t="s">
         <v>131</v>
       </c>
-      <c r="C28" t="s">
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="8" t="s">
+      <c r="B29" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="C29" t="s">
         <v>134</v>
       </c>
-      <c r="C29" t="s">
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="8" t="s">
+      <c r="B30" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="C30" t="s">
         <v>137</v>
       </c>
-      <c r="C30" t="s">
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="8" t="s">
+      <c r="B31" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="C31" t="s">
         <v>140</v>
       </c>
-      <c r="C31" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B32" s="8"/>
       <c r="C32" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="8" t="s">
+      <c r="B33" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="C33" t="s">
         <v>144</v>
       </c>
-      <c r="C33" t="s">
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="8" t="s">
+      <c r="B34" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="C34" t="s">
         <v>147</v>
       </c>
-      <c r="C34" t="s">
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="8" t="s">
+      <c r="B35" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="C35" t="s">
         <v>150</v>
       </c>
-      <c r="C35" t="s">
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="8" t="s">
+      <c r="B36" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="C36" t="s">
         <v>153</v>
       </c>
-      <c r="C36" t="s">
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="8" t="s">
+      <c r="B37" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="C37" t="s">
         <v>156</v>
       </c>
-      <c r="C37" t="s">
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="8" t="s">
+      <c r="B38" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="C38" t="s">
         <v>159</v>
       </c>
-      <c r="C38" t="s">
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="8" t="s">
+      <c r="B39" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="C39" t="s">
         <v>162</v>
       </c>
-      <c r="C39" t="s">
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="8" t="s">
+      <c r="B40" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="C40" t="s">
         <v>165</v>
       </c>
-      <c r="C40" t="s">
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="8" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="8" t="s">
+      <c r="B41" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="B41" s="8" t="s">
+      <c r="C41" t="s">
         <v>168</v>
       </c>
-      <c r="C41" t="s">
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="8" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="8" t="s">
+      <c r="B42" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="C42" t="s">
         <v>171</v>
       </c>
-      <c r="C42" t="s">
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="8" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="8" t="s">
+      <c r="B43" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="B43" s="8" t="s">
+      <c r="C43" t="s">
         <v>174</v>
       </c>
-      <c r="C43" t="s">
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="8" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="8" t="s">
+      <c r="B44" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="B44" s="8" t="s">
+      <c r="C44" t="s">
         <v>177</v>
       </c>
-      <c r="C44" t="s">
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="8" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="8" t="s">
+      <c r="B45" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="B45" s="8" t="s">
+      <c r="C45" t="s">
         <v>180</v>
       </c>
-      <c r="C45" t="s">
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="8" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="8" t="s">
+      <c r="B46" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="B46" s="8" t="s">
+      <c r="C46" t="s">
         <v>183</v>
       </c>
-      <c r="C46" t="s">
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="8" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" s="8" t="s">
+      <c r="B47" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="B47" s="8" t="s">
+      <c r="C47" t="s">
         <v>186</v>
       </c>
-      <c r="C47" t="s">
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="8" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="8" t="s">
+      <c r="B48" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="B48" s="8" t="s">
+      <c r="C48" t="s">
         <v>189</v>
       </c>
-      <c r="C48" t="s">
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="8" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="8" t="s">
+      <c r="B49" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="B49" s="8" t="s">
+      <c r="C49" t="s">
         <v>192</v>
       </c>
-      <c r="C49" t="s">
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="8" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="8" t="s">
+      <c r="B50" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="B50" s="8" t="s">
+      <c r="C50" t="s">
         <v>195</v>
       </c>
-      <c r="C50" t="s">
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="8" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="8" t="s">
+      <c r="B51" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="B51" s="8" t="s">
+      <c r="C51" t="s">
         <v>198</v>
       </c>
-      <c r="C51" t="s">
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="8" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="8" t="s">
+      <c r="B52" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="B52" s="8" t="s">
+      <c r="C52" t="s">
         <v>201</v>
       </c>
-      <c r="C52" t="s">
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="8" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" s="8" t="s">
+      <c r="B53" s="8" t="s">
         <v>203</v>
       </c>
-      <c r="B53" s="8" t="s">
+      <c r="C53" t="s">
         <v>204</v>
       </c>
-      <c r="C53" t="s">
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="8" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" s="8" t="s">
+      <c r="B54" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="B54" s="8" t="s">
+      <c r="C54" t="s">
         <v>207</v>
       </c>
-      <c r="C54" t="s">
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="8" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="A55" s="8" t="s">
+      <c r="B55" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="B55" s="8" t="s">
+      <c r="C55" t="s">
         <v>210</v>
       </c>
-      <c r="C55" t="s">
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="8" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="A56" s="8" t="s">
+      <c r="B56" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="B56" s="8" t="s">
+      <c r="C56" t="s">
         <v>213</v>
       </c>
-      <c r="C56" t="s">
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="8" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" s="8" t="s">
+      <c r="B57" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="B57" s="8" t="s">
+      <c r="C57" t="s">
         <v>216</v>
       </c>
-      <c r="C57" t="s">
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="8" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58" s="8" t="s">
+      <c r="B58" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="B58" s="8" t="s">
+      <c r="C58" t="s">
         <v>219</v>
       </c>
-      <c r="C58" t="s">
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="8" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="A59" s="8" t="s">
+      <c r="B59" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="B59" s="8" t="s">
+      <c r="C59" t="s">
         <v>222</v>
       </c>
-      <c r="C59" t="s">
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="8" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="A60" s="8" t="s">
+      <c r="B60" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="B60" s="8" t="s">
+      <c r="C60" t="s">
         <v>225</v>
       </c>
-      <c r="C60" t="s">
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="8" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" s="8" t="s">
+      <c r="B61" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="B61" s="8" t="s">
+      <c r="C61" t="s">
         <v>228</v>
       </c>
-      <c r="C61" t="s">
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="8" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="A62" s="8" t="s">
+      <c r="B62" s="8" t="s">
         <v>230</v>
       </c>
-      <c r="B62" s="8" t="s">
+      <c r="C62" t="s">
         <v>231</v>
       </c>
-      <c r="C62" t="s">
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="8" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="63" spans="1:3">
-      <c r="A63" s="8" t="s">
+      <c r="B63" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="B63" s="8" t="s">
+      <c r="C63" t="s">
         <v>234</v>
       </c>
-      <c r="C63" t="s">
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="8" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="A64" s="8" t="s">
+      <c r="B64" s="8" t="s">
         <v>236</v>
       </c>
-      <c r="B64" s="8" t="s">
+      <c r="C64" t="s">
         <v>237</v>
       </c>
-      <c r="C64" t="s">
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="8" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="A65" s="8" t="s">
+      <c r="B65" s="8" t="s">
         <v>239</v>
       </c>
-      <c r="B65" s="8" t="s">
+      <c r="C65" t="s">
         <v>240</v>
       </c>
-      <c r="C65" t="s">
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="8" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="A66" s="8" t="s">
+      <c r="B66" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="B66" s="8" t="s">
+      <c r="C66" t="s">
         <v>243</v>
       </c>
-      <c r="C66" t="s">
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="8" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="67" spans="1:3">
-      <c r="A67" s="8" t="s">
+      <c r="B67" s="8" t="s">
         <v>245</v>
       </c>
-      <c r="B67" s="8" t="s">
+      <c r="C67" t="s">
         <v>246</v>
       </c>
-      <c r="C67" t="s">
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="8" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="68" spans="1:3">
-      <c r="A68" s="8" t="s">
+      <c r="B68" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="B68" s="8" t="s">
+      <c r="C68" t="s">
         <v>249</v>
       </c>
-      <c r="C68" t="s">
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="8" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69" s="8" t="s">
+      <c r="B69" s="8" t="s">
         <v>251</v>
       </c>
-      <c r="B69" s="8" t="s">
+      <c r="C69" t="s">
         <v>252</v>
       </c>
-      <c r="C69" t="s">
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="8" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="70" spans="1:3">
-      <c r="A70" s="8" t="s">
+      <c r="B70" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="B70" s="8" t="s">
+      <c r="C70" t="s">
         <v>255</v>
       </c>
-      <c r="C70" t="s">
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="8" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="71" spans="1:3">
-      <c r="A71" s="8" t="s">
+      <c r="B71" s="8" t="s">
         <v>257</v>
       </c>
-      <c r="B71" s="8" t="s">
+      <c r="C71" t="s">
         <v>258</v>
       </c>
-      <c r="C71" t="s">
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="8" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="72" spans="1:3">
-      <c r="A72" s="8" t="s">
+      <c r="B72" s="8" t="s">
         <v>260</v>
       </c>
-      <c r="B72" s="8" t="s">
+      <c r="C72" t="s">
         <v>261</v>
       </c>
-      <c r="C72" t="s">
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="8" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="73" spans="1:3">
-      <c r="A73" s="8" t="s">
+      <c r="B73" s="8" t="s">
         <v>263</v>
       </c>
-      <c r="B73" s="8" t="s">
+      <c r="C73" t="s">
         <v>264</v>
       </c>
-      <c r="C73" t="s">
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="8" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="74" spans="1:3">
-      <c r="A74" s="8" t="s">
+      <c r="B74" s="8" t="s">
         <v>266</v>
       </c>
-      <c r="B74" s="8" t="s">
+      <c r="C74" t="s">
         <v>267</v>
       </c>
-      <c r="C74" t="s">
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="8" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="75" spans="1:3">
-      <c r="A75" s="8" t="s">
+      <c r="B75" s="8" t="s">
         <v>269</v>
       </c>
-      <c r="B75" s="8" t="s">
+      <c r="C75" t="s">
         <v>270</v>
       </c>
-      <c r="C75" t="s">
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="8" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="76" spans="1:3">
-      <c r="A76" s="8" t="s">
+      <c r="B76" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="B76" s="8" t="s">
+      <c r="C76" t="s">
         <v>273</v>
       </c>
-      <c r="C76" t="s">
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="8" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="77" spans="1:3">
-      <c r="A77" s="8" t="s">
+      <c r="B77" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="B77" s="8" t="s">
+      <c r="C77" t="s">
         <v>276</v>
       </c>
-      <c r="C77" t="s">
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="8" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="78" spans="1:3">
-      <c r="A78" s="8" t="s">
+      <c r="B78" s="8" t="s">
         <v>278</v>
       </c>
-      <c r="B78" s="8" t="s">
+      <c r="C78" t="s">
         <v>279</v>
       </c>
-      <c r="C78" t="s">
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="8" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="79" spans="1:3">
-      <c r="A79" s="8" t="s">
+      <c r="B79" s="8" t="s">
         <v>281</v>
       </c>
-      <c r="B79" s="8" t="s">
+      <c r="C79" t="s">
         <v>282</v>
       </c>
-      <c r="C79" t="s">
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="8" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="80" spans="1:3">
-      <c r="A80" s="8" t="s">
+      <c r="B80" s="8" t="s">
         <v>284</v>
       </c>
-      <c r="B80" s="8" t="s">
+      <c r="C80" t="s">
         <v>285</v>
       </c>
-      <c r="C80" t="s">
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="8" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="81" spans="1:3">
-      <c r="A81" s="8" t="s">
+      <c r="B81" s="8" t="s">
         <v>287</v>
       </c>
-      <c r="B81" s="8" t="s">
+      <c r="C81" t="s">
         <v>288</v>
       </c>
-      <c r="C81" t="s">
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="8" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="82" spans="1:3">
-      <c r="A82" s="8" t="s">
+      <c r="B82" s="8" t="s">
         <v>290</v>
       </c>
-      <c r="B82" s="8" t="s">
+      <c r="C82" t="s">
         <v>291</v>
       </c>
-      <c r="C82" t="s">
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="8" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="83" spans="1:3">
-      <c r="A83" s="8" t="s">
+      <c r="B83" s="8" t="s">
         <v>293</v>
       </c>
-      <c r="B83" s="8" t="s">
+      <c r="C83" t="s">
         <v>294</v>
       </c>
-      <c r="C83" t="s">
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="8" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="84" spans="1:3">
-      <c r="A84" s="8" t="s">
+      <c r="B84" s="8" t="s">
         <v>296</v>
       </c>
-      <c r="B84" s="8" t="s">
+      <c r="C84" t="s">
         <v>297</v>
       </c>
-      <c r="C84" t="s">
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="8" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="85" spans="1:3">
-      <c r="A85" s="8" t="s">
+      <c r="B85" s="8" t="s">
         <v>299</v>
       </c>
-      <c r="B85" s="8" t="s">
+      <c r="C85" t="s">
         <v>300</v>
       </c>
-      <c r="C85" t="s">
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="8" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="86" spans="1:3">
-      <c r="A86" s="8" t="s">
+      <c r="B86" s="8" t="s">
         <v>302</v>
       </c>
-      <c r="B86" s="8" t="s">
+      <c r="C86" t="s">
         <v>303</v>
       </c>
-      <c r="C86" t="s">
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="8" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="87" spans="1:3">
-      <c r="A87" s="8" t="s">
+      <c r="B87" s="8" t="s">
         <v>305</v>
       </c>
-      <c r="B87" s="8" t="s">
+      <c r="C87" t="s">
         <v>306</v>
       </c>
-      <c r="C87" t="s">
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="8" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="88" spans="1:3">
-      <c r="A88" s="8" t="s">
+      <c r="B88" s="8" t="s">
         <v>308</v>
       </c>
-      <c r="B88" s="8" t="s">
+      <c r="C88" t="s">
         <v>309</v>
       </c>
-      <c r="C88" t="s">
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="8" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="89" spans="1:3">
-      <c r="A89" s="8" t="s">
+      <c r="B89" s="8" t="s">
         <v>311</v>
       </c>
-      <c r="B89" s="8" t="s">
+      <c r="C89" t="s">
         <v>312</v>
-      </c>
-      <c r="C89" t="s">
-        <v>313</v>
       </c>
     </row>
   </sheetData>
@@ -3119,7 +3112,7 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
     <col min="2" max="2" width="150.5703125" customWidth="1"/>
@@ -3127,297 +3120,297 @@
     <col min="4" max="4" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="13" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="14" t="s">
+        <v>313</v>
+      </c>
+      <c r="D1" s="15"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>314</v>
       </c>
-      <c r="D1" s="18"/>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>315</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="6" t="s">
         <v>316</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>317</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>317</v>
-      </c>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
+      <c r="B3" s="5" t="s">
         <v>318</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="6" t="s">
         <v>319</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>320</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>320</v>
-      </c>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>321</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>323</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>323</v>
-      </c>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>324</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" s="6" t="s">
         <v>325</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="D5" s="6" t="s">
+        <v>325</v>
+      </c>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>326</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>326</v>
-      </c>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
+      <c r="B6" s="5" t="s">
         <v>327</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="6" t="s">
         <v>328</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="D6" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>329</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>329</v>
-      </c>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>330</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="D7" s="6" t="s">
+        <v>331</v>
+      </c>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>332</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>332</v>
-      </c>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>333</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" s="6" t="s">
         <v>334</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="D8" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>335</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>335</v>
-      </c>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
         <v>336</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" s="6" t="s">
         <v>337</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="D9" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>338</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>338</v>
-      </c>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
         <v>339</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" s="6" t="s">
         <v>340</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="D10" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>341</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>341</v>
-      </c>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
         <v>342</v>
       </c>
-      <c r="B11" t="s">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
         <v>344</v>
       </c>
-      <c r="B12" t="s">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
         <v>346</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" s="5"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>347</v>
       </c>
-      <c r="C13" s="5"/>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" t="s">
+      <c r="B15" s="5" t="s">
         <v>348</v>
       </c>
-      <c r="B15" s="5" t="s">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" t="s">
+      <c r="B16" t="s">
         <v>350</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" s="5"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>351</v>
       </c>
-      <c r="C16" s="5"/>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
+      <c r="B17" t="s">
         <v>352</v>
       </c>
-      <c r="B17" t="s">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
+      <c r="B18" s="5" t="s">
         <v>354</v>
       </c>
-      <c r="B18" s="5" t="s">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
+      <c r="B19" t="s">
         <v>356</v>
       </c>
-      <c r="B19" t="s">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
+      <c r="B20" t="s">
         <v>358</v>
       </c>
-      <c r="B20" t="s">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
+      <c r="B21" t="s">
         <v>360</v>
       </c>
-      <c r="B21" t="s">
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s">
+      <c r="B22" t="s">
         <v>362</v>
       </c>
-      <c r="B22" t="s">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s">
+      <c r="B23" t="s">
         <v>364</v>
       </c>
-      <c r="B23" t="s">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s">
+      <c r="B24" t="s">
         <v>366</v>
       </c>
-      <c r="B24" t="s">
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" t="s">
+      <c r="B25" t="s">
         <v>368</v>
       </c>
-      <c r="B25" t="s">
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" t="s">
+      <c r="B26" t="s">
         <v>370</v>
       </c>
-      <c r="B26" t="s">
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" t="s">
+      <c r="B27" t="s">
         <v>372</v>
       </c>
-      <c r="B27" t="s">
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>371</v>
+      </c>
+      <c r="B28" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
-      <c r="A28" t="s">
-        <v>372</v>
-      </c>
-      <c r="B28" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>374</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" t="s">
-        <v>375</v>
       </c>
     </row>
   </sheetData>
@@ -3437,164 +3430,164 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.85546875" customWidth="1"/>
     <col min="2" max="2" width="134.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="14" t="s">
-        <v>314</v>
-      </c>
-      <c r="D1" s="14"/>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="B1" s="15"/>
+      <c r="C1" s="16" t="s">
+        <v>313</v>
+      </c>
+      <c r="D1" s="16"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>376</v>
       </c>
-      <c r="B2" s="10" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="8" t="s">
+      <c r="B3" s="9" t="s">
         <v>378</v>
       </c>
-      <c r="B3" s="9" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="8" t="s">
+      <c r="B4" s="9" t="s">
         <v>380</v>
       </c>
-      <c r="B4" s="9" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="8" t="s">
+      <c r="B5" s="9" t="s">
         <v>382</v>
       </c>
-      <c r="B5" s="9" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="8" t="s">
+      <c r="B6" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="B6" s="9" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="8" t="s">
+      <c r="B7" s="9" t="s">
         <v>386</v>
       </c>
-      <c r="B7" s="9" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="8" t="s">
+      <c r="B8" s="9" t="s">
         <v>388</v>
       </c>
-      <c r="B8" s="9" t="s">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="8" t="s">
+      <c r="B9" s="9" t="s">
         <v>390</v>
       </c>
-      <c r="B9" s="9" t="s">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="8" t="s">
+      <c r="B10" s="9" t="s">
         <v>392</v>
       </c>
-      <c r="B10" s="9" t="s">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="8" t="s">
+      <c r="B11" s="10" t="s">
         <v>394</v>
       </c>
-      <c r="B11" s="10" t="s">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="8" t="s">
+      <c r="B12" s="9" t="s">
         <v>396</v>
       </c>
-      <c r="B12" s="9" t="s">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="8" t="s">
+      <c r="B13" s="9" t="s">
         <v>398</v>
       </c>
-      <c r="B13" s="9" t="s">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="8" t="s">
+      <c r="B14" s="10" t="s">
         <v>400</v>
       </c>
-      <c r="B14" s="10" t="s">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
         <v>401</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="8" t="s">
+      <c r="B15" s="10" t="s">
         <v>402</v>
       </c>
-      <c r="B15" s="10" t="s">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="8" t="s">
+      <c r="B16" s="9" t="s">
         <v>404</v>
       </c>
-      <c r="B16" s="9" t="s">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="8" t="s">
+      <c r="B17" s="9" t="s">
         <v>406</v>
       </c>
-      <c r="B17" s="9" t="s">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="8" t="s">
+      <c r="B18" s="9" t="s">
         <v>408</v>
       </c>
-      <c r="B18" s="9" t="s">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="8" t="s">
+      <c r="B19" s="9" t="s">
         <v>410</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>411</v>
       </c>
     </row>
   </sheetData>
@@ -3610,11 +3603,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" customWidth="1"/>
     <col min="2" max="2" width="40.5703125" customWidth="1"/>
@@ -3622,230 +3615,230 @@
     <col min="4" max="4" width="46.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="15" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="18"/>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="D1" s="15"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>414</v>
-      </c>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="1" t="s">
-        <v>415</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>415</v>
-      </c>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="1" t="s">
-        <v>416</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>416</v>
-      </c>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="1" t="s">
-        <v>417</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>417</v>
-      </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="1" t="s">
-        <v>418</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>418</v>
-      </c>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="1" t="s">
-        <v>419</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>419</v>
       </c>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
         <v>420</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" s="6" t="s">
         <v>421</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="D10" s="7" t="s">
         <v>422</v>
       </c>
-      <c r="D10" s="7" t="s">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>423</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
         <v>424</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" s="6" t="s">
         <v>425</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="D11" s="7" t="s">
         <v>426</v>
       </c>
-      <c r="D11" s="7" t="s">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C12" s="6" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="C12" s="6" t="s">
+      <c r="D12" s="7" t="s">
         <v>428</v>
       </c>
-      <c r="D12" s="7" t="s">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C13" s="6" t="s">
         <v>429</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="C13" s="6" t="s">
+      <c r="D13" s="7" t="s">
         <v>430</v>
       </c>
-      <c r="D13" s="7" t="s">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C14" s="6" t="s">
         <v>431</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="C14" s="6" t="s">
+      <c r="D14" s="7" t="s">
         <v>432</v>
       </c>
-      <c r="D14" s="7" t="s">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C15" s="6" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="C15" s="6" t="s">
+      <c r="D15" s="7" t="s">
         <v>434</v>
       </c>
-      <c r="D15" s="7" t="s">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C16" s="6" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="C16" s="6" t="s">
+      <c r="D16" s="7" t="s">
         <v>436</v>
       </c>
-      <c r="D16" s="7" t="s">
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C17" s="6" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="17" spans="3:4">
-      <c r="C17" s="6" t="s">
+      <c r="D17" s="7" t="s">
         <v>438</v>
       </c>
-      <c r="D17" s="7" t="s">
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C18" s="6" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="18" spans="3:4">
-      <c r="C18" s="6" t="s">
+      <c r="D18" s="7" t="s">
         <v>440</v>
       </c>
-      <c r="D18" s="7" t="s">
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C19" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="19" spans="3:4">
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="7" t="s">
         <v>442</v>
       </c>
-      <c r="D19" s="7" t="s">
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C20" s="1" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="20" spans="3:4">
-      <c r="C20" s="1" t="s">
+      <c r="D20" s="7" t="s">
         <v>444</v>
       </c>
-      <c r="D20" s="7" t="s">
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C21" s="1" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="21" spans="3:4">
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="7" t="s">
         <v>446</v>
       </c>
-      <c r="D21" s="7" t="s">
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C22" s="1" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="22" spans="3:4">
-      <c r="C22" s="1" t="s">
+      <c r="D22" s="7" t="s">
         <v>448</v>
       </c>
-      <c r="D22" s="7" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="28" spans="3:4">
+    </row>
+    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="3:4">
+    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="3:4">
+    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="3:4">
+    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="3:4">
+    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="3:3">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33" s="1"/>
     </row>
   </sheetData>
@@ -3858,26 +3851,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="f1000b3d-15af-42f4-8b30-1751694c7388" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0a44024f-7437-4220-82e3-7a609f3cc5d0">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100AC30A1654071464B83845798603538A6" ma:contentTypeVersion="14" ma:contentTypeDescription="Vytvoří nový dokument" ma:contentTypeScope="" ma:versionID="9168d1d45adf597786ba4404c21a0f63">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f1000b3d-15af-42f4-8b30-1751694c7388" xmlns:ns3="0a44024f-7437-4220-82e3-7a609f3cc5d0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2a603704bc0fe2974ac9a36df3b95205" ns2:_="" ns3:_="">
     <xsd:import namespace="f1000b3d-15af-42f4-8b30-1751694c7388"/>
@@ -4106,14 +4079,60 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="f1000b3d-15af-42f4-8b30-1751694c7388" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0a44024f-7437-4220-82e3-7a609f3cc5d0">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB475825-C6B0-46AE-A469-0210B2AABFAD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4401364-4573-4AA3-A01C-3A51337634B0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f1000b3d-15af-42f4-8b30-1751694c7388"/>
+    <ds:schemaRef ds:uri="0a44024f-7437-4220-82e3-7a609f3cc5d0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20F53162-DA3D-49C7-BB54-6E566081E5DD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20F53162-DA3D-49C7-BB54-6E566081E5DD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4401364-4573-4AA3-A01C-3A51337634B0}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB475825-C6B0-46AE-A469-0210B2AABFAD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f1000b3d-15af-42f4-8b30-1751694c7388"/>
+    <ds:schemaRef ds:uri="0a44024f-7437-4220-82e3-7a609f3cc5d0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
dodělávky, release verze 2.0
</commit_message>
<xml_diff>
--- a/catalogue_manager/Sharepoint_databaze.xlsx
+++ b/catalogue_manager/Sharepoint_databaze.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakub.hlavacek.local\Desktop\JHV\Work\catalogue_manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{999F4B56-2D42-40C9-8BE9-B468CDF41444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="13_ncr:1_{5854EDA4-EDB7-4482-88EE-7784F287C2DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0FDF745-B05A-43DC-A82C-1358DC1737DF}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="3420" windowWidth="28800" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kontrolery" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="450">
   <si>
     <t>Omron FZ/FH</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>FH-5051-10</t>
+  </si>
+  <si>
+    <t>FH vysokorychlostní / vysoce výkonný regulátor, 4 jádra, NPN/PNP, 4 ka</t>
   </si>
   <si>
     <t>FH-5051-20</t>
@@ -1406,7 +1409,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1522,14 +1525,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1539,6 +1540,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1821,11 +1824,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.42578125" customWidth="1"/>
     <col min="2" max="2" width="81.28515625" customWidth="1"/>
@@ -1833,18 +1836,18 @@
     <col min="4" max="4" width="55.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
+      <c r="B1" s="17"/>
       <c r="C1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="12"/>
+      <c r="D1" s="17"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -1859,7 +1862,7 @@
       </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1874,7 +1877,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
@@ -1889,7 +1892,7 @@
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
@@ -1904,7 +1907,7 @@
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
@@ -1919,7 +1922,7 @@
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="4" t="s">
         <v>20</v>
       </c>
@@ -1934,7 +1937,7 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="4" t="s">
         <v>23</v>
       </c>
@@ -1949,7 +1952,7 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="4" t="s">
         <v>26</v>
       </c>
@@ -1964,7 +1967,7 @@
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="4" t="s">
         <v>30</v>
       </c>
@@ -1979,7 +1982,7 @@
       </c>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="4" t="s">
         <v>33</v>
       </c>
@@ -1989,118 +1992,122 @@
       <c r="C11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="4"/>
+      <c r="B12" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="C12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C16" s="1"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C17" s="1"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="4"/>
       <c r="C18" s="1"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C19" s="1"/>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C20" s="1"/>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C21" s="1"/>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C22" s="1"/>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -2116,982 +2123,982 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6243DA3-0875-4C03-8E69-F223C9363894}">
   <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A41" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="24.140625" customWidth="1"/>
     <col min="2" max="2" width="82" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
+      <c r="B1" s="17"/>
       <c r="C1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="12"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D1" s="17"/>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="8" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C10" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C17" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C18" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="8" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="C12" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="C13" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="C14" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="C15" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="C16" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="C17" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="C18" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
-        <v>81</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" s="8" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C20" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" s="8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C21" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" s="8" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C22" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C23" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" s="8" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C24" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" s="8" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C25" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" s="8" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C26" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" s="8" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C27" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" s="8" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C28" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" s="8" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C29" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" s="8" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C30" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" s="8" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C31" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B32" s="8"/>
       <c r="C32" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" s="8" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C33" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34" s="8" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C34" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35" s="8" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C35" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C36" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C37" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38" s="8" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C38" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
       <c r="A39" s="8" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C39" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
       <c r="A40" s="8" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C40" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
       <c r="A41" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C41" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
       <c r="A42" s="8" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C42" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
       <c r="A43" s="8" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C43" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
       <c r="A44" s="8" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C44" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
       <c r="A45" s="8" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C45" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
       <c r="A46" s="8" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C46" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
       <c r="A47" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C47" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
       <c r="A48" s="8" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C48" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
       <c r="A49" s="8" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C49" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
       <c r="A50" s="8" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C50" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
       <c r="A51" s="8" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C51" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
       <c r="A52" s="8" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C52" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
       <c r="A53" s="8" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C53" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
       <c r="A54" s="8" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C54" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
       <c r="A55" s="8" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C55" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
       <c r="A56" s="8" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C56" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
       <c r="A57" s="8" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C57" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
       <c r="A58" s="8" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C58" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
       <c r="A59" s="8" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C59" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
       <c r="A60" s="8" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C60" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
       <c r="A61" s="8" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C61" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
       <c r="A62" s="8" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C62" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
       <c r="A63" s="8" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C63" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
       <c r="A64" s="8" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C64" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
       <c r="A65" s="8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C65" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
       <c r="A66" s="8" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C66" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
       <c r="A67" s="8" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C67" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
       <c r="A68" s="8" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C68" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
       <c r="A69" s="8" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C69" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
       <c r="A70" s="8" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C70" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
       <c r="A71" s="8" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C71" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
       <c r="A72" s="8" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C72" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
       <c r="A73" s="8" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C73" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
       <c r="A74" s="8" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C74" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
       <c r="A75" s="8" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C75" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
       <c r="A76" s="8" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C76" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
       <c r="A77" s="8" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C77" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
       <c r="A78" s="8" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C78" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
       <c r="A79" s="8" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C79" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
       <c r="A80" s="8" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C80" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
       <c r="A81" s="8" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C81" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
       <c r="A82" s="8" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C82" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
       <c r="A83" s="8" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C83" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
       <c r="A84" s="8" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C84" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
       <c r="A85" s="8" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C85" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
       <c r="A86" s="8" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C86" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
       <c r="A87" s="8" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C87" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
       <c r="A88" s="8" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C88" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
       <c r="A89" s="8" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C89" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
   </sheetData>
@@ -3112,7 +3119,7 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
     <col min="2" max="2" width="150.5703125" customWidth="1"/>
@@ -3120,297 +3127,297 @@
     <col min="4" max="4" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="14" t="s">
-        <v>313</v>
-      </c>
-      <c r="D1" s="15"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" s="18"/>
+      <c r="C1" s="13" t="s">
+        <v>314</v>
+      </c>
+      <c r="D1" s="18"/>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B4" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B5" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B7" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B8" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B9" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B10" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B11" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B12" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B13" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B16" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C16" s="5"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B17" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B19" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B20" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B21" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B22" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="B23" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B24" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="B25" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B26" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B27" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>371</v>
-      </c>
       <c r="B28" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
   </sheetData>
@@ -3430,164 +3437,164 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.85546875" customWidth="1"/>
     <col min="2" max="2" width="134.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="16" t="s">
-        <v>313</v>
-      </c>
-      <c r="D1" s="16"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="18"/>
+      <c r="C1" s="14" t="s">
+        <v>314</v>
+      </c>
+      <c r="D1" s="14"/>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="8" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="8" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="8" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="8" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="8" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="8" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="8" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="8" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="8" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="8" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="8" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="8" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="8" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="8" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="8" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" s="8" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18" s="8" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" s="8" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
   </sheetData>
@@ -3603,11 +3610,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.5703125" customWidth="1"/>
     <col min="2" max="2" width="40.5703125" customWidth="1"/>
@@ -3615,230 +3622,230 @@
     <col min="4" max="4" width="46.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:5" ht="15" customHeight="1">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="17" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="15"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D1" s="18"/>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="6" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="B10" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="B11" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="C12" s="6" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="C13" s="6" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="C14" s="6" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="C15" s="6" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="C16" s="6" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4">
       <c r="C17" s="6" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4">
       <c r="C18" s="6" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4">
       <c r="C19" s="1" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4">
       <c r="C20" s="1" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4">
       <c r="C21" s="1" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4">
       <c r="C22" s="1" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="28" spans="3:4">
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:4">
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:4">
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:4">
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:4">
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:3">
       <c r="C33" s="1"/>
     </row>
   </sheetData>
@@ -3851,6 +3858,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="f1000b3d-15af-42f4-8b30-1751694c7388" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0a44024f-7437-4220-82e3-7a609f3cc5d0">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100AC30A1654071464B83845798603538A6" ma:contentTypeVersion="14" ma:contentTypeDescription="Vytvoří nový dokument" ma:contentTypeScope="" ma:versionID="9168d1d45adf597786ba4404c21a0f63">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f1000b3d-15af-42f4-8b30-1751694c7388" xmlns:ns3="0a44024f-7437-4220-82e3-7a609f3cc5d0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2a603704bc0fe2974ac9a36df3b95205" ns2:_="" ns3:_="">
     <xsd:import namespace="f1000b3d-15af-42f4-8b30-1751694c7388"/>
@@ -4079,60 +4106,14 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="f1000b3d-15af-42f4-8b30-1751694c7388" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0a44024f-7437-4220-82e3-7a609f3cc5d0">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4401364-4573-4AA3-A01C-3A51337634B0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="f1000b3d-15af-42f4-8b30-1751694c7388"/>
-    <ds:schemaRef ds:uri="0a44024f-7437-4220-82e3-7a609f3cc5d0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB475825-C6B0-46AE-A469-0210B2AABFAD}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20F53162-DA3D-49C7-BB54-6E566081E5DD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20F53162-DA3D-49C7-BB54-6E566081E5DD}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB475825-C6B0-46AE-A469-0210B2AABFAD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f1000b3d-15af-42f4-8b30-1751694c7388"/>
-    <ds:schemaRef ds:uri="0a44024f-7437-4220-82e3-7a609f3cc5d0"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4401364-4573-4AA3-A01C-3A51337634B0}"/>
 </file>
</xml_diff>